<commit_message>
Cambios y visualizacion del AG
</commit_message>
<xml_diff>
--- a/Trabajo Practico Integrador/Salidas/Datos.xlsx
+++ b/Trabajo Practico Integrador/Salidas/Datos.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Generacion 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Generacion 2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,327 +413,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Poblacion</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Min. Func. Objetivo</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Max. Func. Objetivo</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Media Func. Objetivo</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>39357</v>
-      </c>
-      <c r="C2" t="n">
-        <v>44081</v>
-      </c>
-      <c r="D2" t="n">
-        <v>41625.4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>38007</v>
-      </c>
-      <c r="C3" t="n">
-        <v>43747</v>
-      </c>
-      <c r="D3" t="n">
-        <v>40907</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>32629</v>
-      </c>
-      <c r="C4" t="n">
-        <v>41002</v>
-      </c>
-      <c r="D4" t="n">
-        <v>37792.6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>40815</v>
-      </c>
-      <c r="C5" t="n">
-        <v>44406</v>
-      </c>
-      <c r="D5" t="n">
-        <v>43023.4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>33813</v>
-      </c>
-      <c r="C6" t="n">
-        <v>43847</v>
-      </c>
-      <c r="D6" t="n">
-        <v>41196.4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>39806</v>
-      </c>
-      <c r="C7" t="n">
-        <v>42843</v>
-      </c>
-      <c r="D7" t="n">
-        <v>41493</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>39033</v>
-      </c>
-      <c r="C8" t="n">
-        <v>42872</v>
-      </c>
-      <c r="D8" t="n">
-        <v>41078.8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>35236</v>
-      </c>
-      <c r="C9" t="n">
-        <v>41534</v>
-      </c>
-      <c r="D9" t="n">
-        <v>38899.4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>39168</v>
-      </c>
-      <c r="C10" t="n">
-        <v>43785</v>
-      </c>
-      <c r="D10" t="n">
-        <v>41753.2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>39757</v>
-      </c>
-      <c r="C11" t="n">
-        <v>43277</v>
-      </c>
-      <c r="D11" t="n">
-        <v>42117.2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="n">
-        <v>39333</v>
-      </c>
-      <c r="C12" t="n">
-        <v>43551</v>
-      </c>
-      <c r="D12" t="n">
-        <v>41355.2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="n">
-        <v>38637</v>
-      </c>
-      <c r="C13" t="n">
-        <v>41423</v>
-      </c>
-      <c r="D13" t="n">
-        <v>40625.2</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="n">
-        <v>40877</v>
-      </c>
-      <c r="C14" t="n">
-        <v>43796</v>
-      </c>
-      <c r="D14" t="n">
-        <v>42327.8</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="n">
-        <v>37031</v>
-      </c>
-      <c r="C15" t="n">
-        <v>43228</v>
-      </c>
-      <c r="D15" t="n">
-        <v>40899.6</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="n">
-        <v>38328</v>
-      </c>
-      <c r="C16" t="n">
-        <v>42903</v>
-      </c>
-      <c r="D16" t="n">
-        <v>40513.4</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="n">
-        <v>39960</v>
-      </c>
-      <c r="C17" t="n">
-        <v>44103</v>
-      </c>
-      <c r="D17" t="n">
-        <v>42230.4</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="n">
-        <v>38707</v>
-      </c>
-      <c r="C18" t="n">
-        <v>44103</v>
-      </c>
-      <c r="D18" t="n">
-        <v>41476.6</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="n">
-        <v>40298</v>
-      </c>
-      <c r="C19" t="n">
-        <v>44940</v>
-      </c>
-      <c r="D19" t="n">
-        <v>43152.4</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="n">
-        <v>36200</v>
-      </c>
-      <c r="C20" t="n">
-        <v>43021</v>
-      </c>
-      <c r="D20" t="n">
-        <v>39292.6</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="n">
-        <v>38669</v>
-      </c>
-      <c r="C21" t="n">
-        <v>41830</v>
-      </c>
-      <c r="D21" t="n">
-        <v>40517.8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -770,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>38392</v>
+        <v>37421</v>
       </c>
       <c r="C2" t="n">
-        <v>43500</v>
+        <v>43197</v>
       </c>
       <c r="D2" t="n">
-        <v>39891</v>
+        <v>41183</v>
       </c>
     </row>
     <row r="3">
@@ -784,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>40292</v>
+        <v>43197</v>
       </c>
       <c r="C3" t="n">
-        <v>44130</v>
+        <v>43796</v>
       </c>
       <c r="D3" t="n">
-        <v>41752.2</v>
+        <v>43484.25</v>
       </c>
     </row>
     <row r="4">
@@ -798,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>38707</v>
+        <v>41062</v>
       </c>
       <c r="C4" t="n">
-        <v>44103</v>
+        <v>44348</v>
       </c>
       <c r="D4" t="n">
-        <v>41656.4</v>
+        <v>43119.75</v>
       </c>
     </row>
     <row r="5">
@@ -812,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>34937</v>
+        <v>44348</v>
       </c>
       <c r="C5" t="n">
-        <v>40641</v>
+        <v>44733</v>
       </c>
       <c r="D5" t="n">
-        <v>38187.8</v>
+        <v>44540.5</v>
       </c>
     </row>
     <row r="6">
@@ -826,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>37276</v>
+        <v>42933</v>
       </c>
       <c r="C6" t="n">
-        <v>44395</v>
+        <v>46137</v>
       </c>
       <c r="D6" t="n">
-        <v>41043.4</v>
+        <v>44634</v>
       </c>
     </row>
     <row r="7">
@@ -840,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>39614</v>
+        <v>44070</v>
       </c>
       <c r="C7" t="n">
-        <v>44419</v>
+        <v>46533</v>
       </c>
       <c r="D7" t="n">
-        <v>41931.8</v>
+        <v>45429.75</v>
       </c>
     </row>
     <row r="8">
@@ -854,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>39076</v>
+        <v>45558</v>
       </c>
       <c r="C8" t="n">
-        <v>44978</v>
+        <v>46533</v>
       </c>
       <c r="D8" t="n">
-        <v>41641.6</v>
+        <v>46289.25</v>
       </c>
     </row>
     <row r="9">
@@ -868,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>38967</v>
+        <v>45618</v>
       </c>
       <c r="C9" t="n">
-        <v>44141</v>
+        <v>45618</v>
       </c>
       <c r="D9" t="n">
-        <v>41721.2</v>
+        <v>45618</v>
       </c>
     </row>
     <row r="10">
@@ -882,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>39399</v>
+        <v>45618</v>
       </c>
       <c r="C10" t="n">
-        <v>42565</v>
+        <v>46277</v>
       </c>
       <c r="D10" t="n">
-        <v>41436.4</v>
+        <v>45947.5</v>
       </c>
     </row>
     <row r="11">
@@ -896,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>36326</v>
+        <v>42608</v>
       </c>
       <c r="C11" t="n">
-        <v>43778</v>
+        <v>46847</v>
       </c>
       <c r="D11" t="n">
-        <v>39916</v>
+        <v>45273.5</v>
       </c>
     </row>
     <row r="12">
@@ -910,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>38003</v>
+        <v>41144</v>
       </c>
       <c r="C12" t="n">
-        <v>42253</v>
+        <v>47142</v>
       </c>
       <c r="D12" t="n">
-        <v>40424.8</v>
+        <v>44981.25</v>
       </c>
     </row>
     <row r="13">
@@ -924,13 +602,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>34488</v>
+        <v>47142</v>
       </c>
       <c r="C13" t="n">
-        <v>43807</v>
+        <v>47142</v>
       </c>
       <c r="D13" t="n">
-        <v>40828.2</v>
+        <v>47142</v>
       </c>
     </row>
     <row r="14">
@@ -938,13 +616,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>36968</v>
+        <v>47142</v>
       </c>
       <c r="C14" t="n">
-        <v>42191</v>
+        <v>47142</v>
       </c>
       <c r="D14" t="n">
-        <v>39753.4</v>
+        <v>47142</v>
       </c>
     </row>
     <row r="15">
@@ -952,13 +630,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>40209</v>
+        <v>47142</v>
       </c>
       <c r="C15" t="n">
-        <v>43126</v>
+        <v>48026</v>
       </c>
       <c r="D15" t="n">
-        <v>41360.8</v>
+        <v>47363</v>
       </c>
     </row>
     <row r="16">
@@ -966,13 +644,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>36689</v>
+        <v>45342</v>
       </c>
       <c r="C16" t="n">
-        <v>43827</v>
+        <v>48877</v>
       </c>
       <c r="D16" t="n">
-        <v>40909</v>
+        <v>47346.75</v>
       </c>
     </row>
     <row r="17">
@@ -980,13 +658,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>37576</v>
+        <v>43167</v>
       </c>
       <c r="C17" t="n">
-        <v>44081</v>
+        <v>52276</v>
       </c>
       <c r="D17" t="n">
-        <v>41884.2</v>
+        <v>47588.75</v>
       </c>
     </row>
     <row r="18">
@@ -994,13 +672,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>38869</v>
+        <v>45342</v>
       </c>
       <c r="C18" t="n">
-        <v>44929</v>
+        <v>53561</v>
       </c>
       <c r="D18" t="n">
-        <v>40949.2</v>
+        <v>50233.5</v>
       </c>
     </row>
     <row r="19">
@@ -1008,13 +686,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>36703</v>
+        <v>45342</v>
       </c>
       <c r="C19" t="n">
-        <v>44032</v>
+        <v>53561</v>
       </c>
       <c r="D19" t="n">
-        <v>41127</v>
+        <v>50215.75</v>
       </c>
     </row>
     <row r="20">
@@ -1022,13 +700,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>38319</v>
+        <v>49955</v>
       </c>
       <c r="C20" t="n">
-        <v>42006</v>
+        <v>53561</v>
       </c>
       <c r="D20" t="n">
-        <v>39974.4</v>
+        <v>51840.25</v>
       </c>
     </row>
     <row r="21">
@@ -1036,13 +714,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>38110</v>
+        <v>49171</v>
       </c>
       <c r="C21" t="n">
-        <v>44662</v>
+        <v>53561</v>
       </c>
       <c r="D21" t="n">
-        <v>40770.2</v>
+        <v>50825</v>
       </c>
     </row>
     <row r="22">
@@ -1050,13 +728,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>39441</v>
+        <v>49440</v>
       </c>
       <c r="C22" t="n">
-        <v>42892</v>
+        <v>53561</v>
       </c>
       <c r="D22" t="n">
-        <v>40402</v>
+        <v>52444</v>
       </c>
     </row>
     <row r="23">
@@ -1064,13 +742,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>37650</v>
+        <v>53561</v>
       </c>
       <c r="C23" t="n">
-        <v>40837</v>
+        <v>53561</v>
       </c>
       <c r="D23" t="n">
-        <v>39281.8</v>
+        <v>53561</v>
       </c>
     </row>
     <row r="24">
@@ -1078,13 +756,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>41111</v>
+        <v>53561</v>
       </c>
       <c r="C24" t="n">
-        <v>44858</v>
+        <v>53561</v>
       </c>
       <c r="D24" t="n">
-        <v>42844.4</v>
+        <v>53561</v>
       </c>
     </row>
     <row r="25">
@@ -1092,13 +770,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>34449</v>
+        <v>51761</v>
       </c>
       <c r="C25" t="n">
-        <v>44032</v>
+        <v>55361</v>
       </c>
       <c r="D25" t="n">
-        <v>40454</v>
+        <v>53561</v>
       </c>
     </row>
     <row r="26">
@@ -1106,13 +784,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>36868</v>
+        <v>53561</v>
       </c>
       <c r="C26" t="n">
-        <v>42351</v>
+        <v>55361</v>
       </c>
       <c r="D26" t="n">
-        <v>40092.4</v>
+        <v>54911</v>
       </c>
     </row>
     <row r="27">
@@ -1120,13 +798,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>36959</v>
+        <v>55361</v>
       </c>
       <c r="C27" t="n">
-        <v>40020</v>
+        <v>56151</v>
       </c>
       <c r="D27" t="n">
-        <v>38340.2</v>
+        <v>55953.5</v>
       </c>
     </row>
     <row r="28">
@@ -1134,13 +812,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>36921</v>
+        <v>56151</v>
       </c>
       <c r="C28" t="n">
-        <v>43502</v>
+        <v>56151</v>
       </c>
       <c r="D28" t="n">
-        <v>40525</v>
+        <v>56151</v>
       </c>
     </row>
     <row r="29">
@@ -1148,13 +826,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>39791</v>
+        <v>54675</v>
       </c>
       <c r="C29" t="n">
-        <v>42794</v>
+        <v>56151</v>
       </c>
       <c r="D29" t="n">
-        <v>41495.2</v>
+        <v>55782</v>
       </c>
     </row>
     <row r="30">
@@ -1162,13 +840,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>39615</v>
+        <v>52562</v>
       </c>
       <c r="C30" t="n">
-        <v>44624</v>
+        <v>56198</v>
       </c>
       <c r="D30" t="n">
-        <v>42729</v>
+        <v>55265.5</v>
       </c>
     </row>
     <row r="31">
@@ -1176,13 +854,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>38007</v>
+        <v>55099</v>
       </c>
       <c r="C31" t="n">
-        <v>44063</v>
+        <v>57703</v>
       </c>
       <c r="D31" t="n">
-        <v>41205.6</v>
+        <v>56300.75</v>
       </c>
     </row>
     <row r="32">
@@ -1190,13 +868,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>37887</v>
+        <v>55099</v>
       </c>
       <c r="C32" t="n">
-        <v>43442</v>
+        <v>56250</v>
       </c>
       <c r="D32" t="n">
-        <v>40795.2</v>
+        <v>55750</v>
       </c>
     </row>
     <row r="33">
@@ -1204,13 +882,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>35992</v>
+        <v>54559</v>
       </c>
       <c r="C33" t="n">
-        <v>42373</v>
+        <v>56250</v>
       </c>
       <c r="D33" t="n">
-        <v>38564</v>
+        <v>55489.75</v>
       </c>
     </row>
     <row r="34">
@@ -1218,13 +896,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>36966</v>
+        <v>55154</v>
       </c>
       <c r="C34" t="n">
-        <v>43524</v>
+        <v>56250</v>
       </c>
       <c r="D34" t="n">
-        <v>41464.4</v>
+        <v>55976</v>
       </c>
     </row>
     <row r="35">
@@ -1232,13 +910,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>38711</v>
+        <v>52385</v>
       </c>
       <c r="C35" t="n">
-        <v>43698</v>
+        <v>56964</v>
       </c>
       <c r="D35" t="n">
-        <v>41714.4</v>
+        <v>54914.25</v>
       </c>
     </row>
     <row r="36">
@@ -1246,13 +924,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>36620</v>
+        <v>55292</v>
       </c>
       <c r="C36" t="n">
-        <v>40842</v>
+        <v>56964</v>
       </c>
       <c r="D36" t="n">
-        <v>39014.2</v>
+        <v>56546</v>
       </c>
     </row>
     <row r="37">
@@ -1260,13 +938,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>36749</v>
+        <v>56964</v>
       </c>
       <c r="C37" t="n">
-        <v>44130</v>
+        <v>58135</v>
       </c>
       <c r="D37" t="n">
-        <v>40423.4</v>
+        <v>57256.75</v>
       </c>
     </row>
     <row r="38">
@@ -1274,13 +952,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>36491</v>
+        <v>55508</v>
       </c>
       <c r="C38" t="n">
-        <v>44406</v>
+        <v>56964</v>
       </c>
       <c r="D38" t="n">
-        <v>38887.6</v>
+        <v>56600</v>
       </c>
     </row>
     <row r="39">
@@ -1288,13 +966,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>37301</v>
+        <v>55508</v>
       </c>
       <c r="C39" t="n">
-        <v>42881</v>
+        <v>56964</v>
       </c>
       <c r="D39" t="n">
-        <v>40691.6</v>
+        <v>56236</v>
       </c>
     </row>
     <row r="40">
@@ -1302,13 +980,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>33598</v>
+        <v>53875</v>
       </c>
       <c r="C40" t="n">
-        <v>44602</v>
+        <v>57197</v>
       </c>
       <c r="D40" t="n">
-        <v>39777.8</v>
+        <v>56250</v>
       </c>
     </row>
     <row r="41">
@@ -1316,13 +994,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>36651</v>
+        <v>55295</v>
       </c>
       <c r="C41" t="n">
-        <v>42943</v>
+        <v>57197</v>
       </c>
       <c r="D41" t="n">
-        <v>40006.8</v>
+        <v>56555.25</v>
       </c>
     </row>
     <row r="42">
@@ -1330,13 +1008,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>37813</v>
+        <v>57197</v>
       </c>
       <c r="C42" t="n">
-        <v>44940</v>
+        <v>57197</v>
       </c>
       <c r="D42" t="n">
-        <v>41455</v>
+        <v>57197</v>
       </c>
     </row>
     <row r="43">
@@ -1344,13 +1022,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>37280</v>
+        <v>55527</v>
       </c>
       <c r="C43" t="n">
-        <v>42832</v>
+        <v>57197</v>
       </c>
       <c r="D43" t="n">
-        <v>40848.8</v>
+        <v>56779.5</v>
       </c>
     </row>
     <row r="44">
@@ -1358,13 +1036,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>40040</v>
+        <v>56295</v>
       </c>
       <c r="C44" t="n">
-        <v>44733</v>
+        <v>57197</v>
       </c>
       <c r="D44" t="n">
-        <v>41583.6</v>
+        <v>56971.5</v>
       </c>
     </row>
     <row r="45">
@@ -1372,13 +1050,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>35447</v>
+        <v>57197</v>
       </c>
       <c r="C45" t="n">
-        <v>40439</v>
+        <v>57442</v>
       </c>
       <c r="D45" t="n">
-        <v>38700.8</v>
+        <v>57258.25</v>
       </c>
     </row>
     <row r="46">
@@ -1386,13 +1064,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>39782</v>
+        <v>55224</v>
       </c>
       <c r="C46" t="n">
-        <v>44408</v>
+        <v>58183</v>
       </c>
       <c r="D46" t="n">
-        <v>41949.2</v>
+        <v>56535</v>
       </c>
     </row>
     <row r="47">
@@ -1400,13 +1078,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>39497</v>
+        <v>55350</v>
       </c>
       <c r="C47" t="n">
-        <v>41894</v>
+        <v>58427</v>
       </c>
       <c r="D47" t="n">
-        <v>40885.2</v>
+        <v>57535.75</v>
       </c>
     </row>
     <row r="48">
@@ -1414,13 +1092,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>36995</v>
+        <v>57358</v>
       </c>
       <c r="C48" t="n">
-        <v>42941</v>
+        <v>58427</v>
       </c>
       <c r="D48" t="n">
-        <v>40255.6</v>
+        <v>57831.5</v>
       </c>
     </row>
     <row r="49">
@@ -1428,13 +1106,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>38277</v>
+        <v>53965</v>
       </c>
       <c r="C49" t="n">
-        <v>43411</v>
+        <v>59190</v>
       </c>
       <c r="D49" t="n">
-        <v>41083.2</v>
+        <v>57502.25</v>
       </c>
     </row>
     <row r="50">
@@ -1442,13 +1120,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>41427</v>
+        <v>57053</v>
       </c>
       <c r="C50" t="n">
-        <v>44419</v>
+        <v>59190</v>
       </c>
       <c r="D50" t="n">
-        <v>42666.6</v>
+        <v>58274.25</v>
       </c>
     </row>
     <row r="51">
@@ -1456,13 +1134,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>36491</v>
+        <v>50790</v>
       </c>
       <c r="C51" t="n">
-        <v>42008</v>
+        <v>61145</v>
       </c>
       <c r="D51" t="n">
-        <v>40011</v>
+        <v>57092.5</v>
       </c>
     </row>
     <row r="52">
@@ -1470,13 +1148,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>39858</v>
+        <v>55566</v>
       </c>
       <c r="C52" t="n">
-        <v>44406</v>
+        <v>59045</v>
       </c>
       <c r="D52" t="n">
-        <v>42242.4</v>
+        <v>57855</v>
       </c>
     </row>
     <row r="53">
@@ -1484,13 +1162,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>35754</v>
+        <v>59045</v>
       </c>
       <c r="C53" t="n">
-        <v>44466</v>
+        <v>59194</v>
       </c>
       <c r="D53" t="n">
-        <v>40825.2</v>
+        <v>59119.5</v>
       </c>
     </row>
     <row r="54">
@@ -1498,13 +1176,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>39735</v>
+        <v>56148</v>
       </c>
       <c r="C54" t="n">
-        <v>42607</v>
+        <v>59194</v>
       </c>
       <c r="D54" t="n">
-        <v>40919</v>
+        <v>57836.25</v>
       </c>
     </row>
     <row r="55">
@@ -1512,13 +1190,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>37680</v>
+        <v>57241</v>
       </c>
       <c r="C55" t="n">
-        <v>43767</v>
+        <v>59194</v>
       </c>
       <c r="D55" t="n">
-        <v>41965.4</v>
+        <v>58632.25</v>
       </c>
     </row>
     <row r="56">
@@ -1526,13 +1204,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>36605</v>
+        <v>59194</v>
       </c>
       <c r="C56" t="n">
-        <v>43493</v>
+        <v>59194</v>
       </c>
       <c r="D56" t="n">
-        <v>41150.2</v>
+        <v>59194</v>
       </c>
     </row>
     <row r="57">
@@ -1540,13 +1218,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>39430</v>
+        <v>57729</v>
       </c>
       <c r="C57" t="n">
-        <v>44673</v>
+        <v>59194</v>
       </c>
       <c r="D57" t="n">
-        <v>41805</v>
+        <v>58827.75</v>
       </c>
     </row>
     <row r="58">
@@ -1554,13 +1232,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>39461</v>
+        <v>59194</v>
       </c>
       <c r="C58" t="n">
-        <v>44967</v>
+        <v>59194</v>
       </c>
       <c r="D58" t="n">
-        <v>40978</v>
+        <v>59194</v>
       </c>
     </row>
     <row r="59">
@@ -1568,13 +1246,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>38068</v>
+        <v>59194</v>
       </c>
       <c r="C59" t="n">
-        <v>44052</v>
+        <v>59866</v>
       </c>
       <c r="D59" t="n">
-        <v>41238</v>
+        <v>59362</v>
       </c>
     </row>
     <row r="60">
@@ -1582,13 +1260,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>37516</v>
+        <v>56520</v>
       </c>
       <c r="C60" t="n">
-        <v>42142</v>
+        <v>61456</v>
       </c>
       <c r="D60" t="n">
-        <v>39896.6</v>
+        <v>58988.5</v>
       </c>
     </row>
     <row r="61">
@@ -1596,13 +1274,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>40928</v>
+        <v>58989</v>
       </c>
       <c r="C61" t="n">
-        <v>43707</v>
+        <v>61456</v>
       </c>
       <c r="D61" t="n">
-        <v>42285.6</v>
+        <v>59605.75</v>
       </c>
     </row>
     <row r="62">
@@ -1610,13 +1288,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>40461</v>
+        <v>55665</v>
       </c>
       <c r="C62" t="n">
-        <v>43582</v>
+        <v>61456</v>
       </c>
       <c r="D62" t="n">
-        <v>42070.6</v>
+        <v>58774.75</v>
       </c>
     </row>
     <row r="63">
@@ -1624,13 +1302,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>35456</v>
+        <v>56082</v>
       </c>
       <c r="C63" t="n">
-        <v>40594</v>
+        <v>61456</v>
       </c>
       <c r="D63" t="n">
-        <v>38924.2</v>
+        <v>59700.75</v>
       </c>
     </row>
     <row r="64">
@@ -1638,13 +1316,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>35764</v>
+        <v>60015</v>
       </c>
       <c r="C64" t="n">
-        <v>44477</v>
+        <v>61763</v>
       </c>
       <c r="D64" t="n">
-        <v>40077.8</v>
+        <v>61172.5</v>
       </c>
     </row>
     <row r="65">
@@ -1652,13 +1330,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>39227</v>
+        <v>58063</v>
       </c>
       <c r="C65" t="n">
-        <v>43747</v>
+        <v>60015</v>
       </c>
       <c r="D65" t="n">
-        <v>41144</v>
+        <v>59363</v>
       </c>
     </row>
     <row r="66">
@@ -1666,13 +1344,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>36494</v>
+        <v>56001</v>
       </c>
       <c r="C66" t="n">
-        <v>43482</v>
+        <v>60015</v>
       </c>
       <c r="D66" t="n">
-        <v>40008.4</v>
+        <v>58306</v>
       </c>
     </row>
     <row r="67">
@@ -1680,13 +1358,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>35627</v>
+        <v>57471</v>
       </c>
       <c r="C67" t="n">
-        <v>42006</v>
+        <v>60015</v>
       </c>
       <c r="D67" t="n">
-        <v>39839.8</v>
+        <v>59309.5</v>
       </c>
     </row>
     <row r="68">
@@ -1694,13 +1372,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>39054</v>
+        <v>56281</v>
       </c>
       <c r="C68" t="n">
-        <v>43502</v>
+        <v>60015</v>
       </c>
       <c r="D68" t="n">
-        <v>41154.2</v>
+        <v>58445.5</v>
       </c>
     </row>
     <row r="69">
@@ -1708,13 +1386,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>39370</v>
+        <v>57338</v>
       </c>
       <c r="C69" t="n">
-        <v>41854</v>
+        <v>60015</v>
       </c>
       <c r="D69" t="n">
-        <v>40691.8</v>
+        <v>58344.25</v>
       </c>
     </row>
     <row r="70">
@@ -1722,13 +1400,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>39056</v>
+        <v>56531</v>
       </c>
       <c r="C70" t="n">
-        <v>43442</v>
+        <v>60015</v>
       </c>
       <c r="D70" t="n">
-        <v>41081.4</v>
+        <v>58215.75</v>
       </c>
     </row>
     <row r="71">
@@ -1736,13 +1414,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>36940</v>
+        <v>58137</v>
       </c>
       <c r="C71" t="n">
-        <v>44337</v>
+        <v>59253</v>
       </c>
       <c r="D71" t="n">
-        <v>40714</v>
+        <v>58522.5</v>
       </c>
     </row>
     <row r="72">
@@ -1750,13 +1428,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>36797</v>
+        <v>58055</v>
       </c>
       <c r="C72" t="n">
-        <v>42761</v>
+        <v>59253</v>
       </c>
       <c r="D72" t="n">
-        <v>39469.6</v>
+        <v>58448.75</v>
       </c>
     </row>
     <row r="73">
@@ -1764,13 +1442,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>38410</v>
+        <v>58034</v>
       </c>
       <c r="C73" t="n">
-        <v>42654</v>
+        <v>59032</v>
       </c>
       <c r="D73" t="n">
-        <v>41158.6</v>
+        <v>58441.5</v>
       </c>
     </row>
     <row r="74">
@@ -1778,13 +1456,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>36921</v>
+        <v>55970</v>
       </c>
       <c r="C74" t="n">
-        <v>43126</v>
+        <v>61366</v>
       </c>
       <c r="D74" t="n">
-        <v>40642.2</v>
+        <v>58259.75</v>
       </c>
     </row>
     <row r="75">
@@ -1792,13 +1470,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>39054</v>
+        <v>56263</v>
       </c>
       <c r="C75" t="n">
-        <v>44651</v>
+        <v>59396</v>
       </c>
       <c r="D75" t="n">
-        <v>42465.6</v>
+        <v>57792.5</v>
       </c>
     </row>
     <row r="76">
@@ -1806,13 +1484,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>36437</v>
+        <v>57468</v>
       </c>
       <c r="C76" t="n">
-        <v>44673</v>
+        <v>59396</v>
       </c>
       <c r="D76" t="n">
-        <v>41333.4</v>
+        <v>58212</v>
       </c>
     </row>
     <row r="77">
@@ -1820,13 +1498,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>39399</v>
+        <v>55234</v>
       </c>
       <c r="C77" t="n">
-        <v>44348</v>
+        <v>59396</v>
       </c>
       <c r="D77" t="n">
-        <v>42215.8</v>
+        <v>57773.5</v>
       </c>
     </row>
     <row r="78">
@@ -1834,13 +1512,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>35800</v>
+        <v>57622</v>
       </c>
       <c r="C78" t="n">
-        <v>43598</v>
+        <v>60100</v>
       </c>
       <c r="D78" t="n">
-        <v>39642.2</v>
+        <v>58546.5</v>
       </c>
     </row>
     <row r="79">
@@ -1848,13 +1526,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>38739</v>
+        <v>57923</v>
       </c>
       <c r="C79" t="n">
-        <v>42026</v>
+        <v>59431</v>
       </c>
       <c r="D79" t="n">
-        <v>40743.4</v>
+        <v>58467</v>
       </c>
     </row>
     <row r="80">
@@ -1862,13 +1540,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>40418</v>
+        <v>58257</v>
       </c>
       <c r="C80" t="n">
-        <v>44092</v>
+        <v>59431</v>
       </c>
       <c r="D80" t="n">
-        <v>41775.6</v>
+        <v>59137.5</v>
       </c>
     </row>
     <row r="81">
@@ -1876,13 +1554,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>34713</v>
+        <v>59431</v>
       </c>
       <c r="C81" t="n">
-        <v>43255</v>
+        <v>59431</v>
       </c>
       <c r="D81" t="n">
-        <v>39054</v>
+        <v>59431</v>
       </c>
     </row>
     <row r="82">
@@ -1890,13 +1568,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>39289</v>
+        <v>59431</v>
       </c>
       <c r="C82" t="n">
-        <v>44150</v>
+        <v>59431</v>
       </c>
       <c r="D82" t="n">
-        <v>41850</v>
+        <v>59431</v>
       </c>
     </row>
     <row r="83">
@@ -1904,13 +1582,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>37578</v>
+        <v>59431</v>
       </c>
       <c r="C83" t="n">
-        <v>43769</v>
+        <v>60270</v>
       </c>
       <c r="D83" t="n">
-        <v>40519.4</v>
+        <v>59990.75</v>
       </c>
     </row>
     <row r="84">
@@ -1918,13 +1596,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>39270</v>
+        <v>57369</v>
       </c>
       <c r="C84" t="n">
-        <v>44613</v>
+        <v>60740</v>
       </c>
       <c r="D84" t="n">
-        <v>41800.2</v>
+        <v>59662.25</v>
       </c>
     </row>
     <row r="85">
@@ -1932,13 +1610,13 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>36867</v>
+        <v>58470</v>
       </c>
       <c r="C85" t="n">
-        <v>43006</v>
+        <v>62540</v>
       </c>
       <c r="D85" t="n">
-        <v>39924.8</v>
+        <v>60622.5</v>
       </c>
     </row>
     <row r="86">
@@ -1946,13 +1624,13 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>36167</v>
+        <v>57950</v>
       </c>
       <c r="C86" t="n">
-        <v>42892</v>
+        <v>62540</v>
       </c>
       <c r="D86" t="n">
-        <v>39858.6</v>
+        <v>59588</v>
       </c>
     </row>
     <row r="87">
@@ -1960,13 +1638,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>35785</v>
+        <v>57950</v>
       </c>
       <c r="C87" t="n">
-        <v>44141</v>
+        <v>62540</v>
       </c>
       <c r="D87" t="n">
-        <v>39275.8</v>
+        <v>60637.75</v>
       </c>
     </row>
     <row r="88">
@@ -1974,13 +1652,13 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>37479</v>
+        <v>59521</v>
       </c>
       <c r="C88" t="n">
-        <v>40868</v>
+        <v>62540</v>
       </c>
       <c r="D88" t="n">
-        <v>38687.4</v>
+        <v>60992</v>
       </c>
     </row>
     <row r="89">
@@ -1988,13 +1666,13 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>33007</v>
+        <v>61167</v>
       </c>
       <c r="C89" t="n">
-        <v>43725</v>
+        <v>62540</v>
       </c>
       <c r="D89" t="n">
-        <v>40791.8</v>
+        <v>61510.25</v>
       </c>
     </row>
     <row r="90">
@@ -2002,13 +1680,13 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>39256</v>
+        <v>60671</v>
       </c>
       <c r="C90" t="n">
-        <v>44602</v>
+        <v>62825</v>
       </c>
       <c r="D90" t="n">
-        <v>42587.4</v>
+        <v>61872</v>
       </c>
     </row>
     <row r="91">
@@ -2016,13 +1694,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>40182</v>
+        <v>58798</v>
       </c>
       <c r="C91" t="n">
-        <v>43088</v>
+        <v>62825</v>
       </c>
       <c r="D91" t="n">
-        <v>41545.6</v>
+        <v>61251.25</v>
       </c>
     </row>
     <row r="92">
@@ -2030,13 +1708,13 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>38894</v>
+        <v>61474</v>
       </c>
       <c r="C92" t="n">
-        <v>44978</v>
+        <v>63502</v>
       </c>
       <c r="D92" t="n">
-        <v>40908.4</v>
+        <v>62656.5</v>
       </c>
     </row>
     <row r="93">
@@ -2044,13 +1722,13 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>35809</v>
+        <v>62825</v>
       </c>
       <c r="C93" t="n">
-        <v>39858</v>
+        <v>62825</v>
       </c>
       <c r="D93" t="n">
-        <v>38474.4</v>
+        <v>62825</v>
       </c>
     </row>
     <row r="94">
@@ -2058,13 +1736,13 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>39125</v>
+        <v>62019</v>
       </c>
       <c r="C94" t="n">
-        <v>44477</v>
+        <v>63101</v>
       </c>
       <c r="D94" t="n">
-        <v>41948.4</v>
+        <v>62692.5</v>
       </c>
     </row>
     <row r="95">
@@ -2072,13 +1750,13 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>35389</v>
+        <v>62825</v>
       </c>
       <c r="C95" t="n">
-        <v>43079</v>
+        <v>63101</v>
       </c>
       <c r="D95" t="n">
-        <v>40040.4</v>
+        <v>62963</v>
       </c>
     </row>
     <row r="96">
@@ -2086,13 +1764,13 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>39515</v>
+        <v>59626</v>
       </c>
       <c r="C96" t="n">
-        <v>43155</v>
+        <v>63101</v>
       </c>
       <c r="D96" t="n">
-        <v>41448.6</v>
+        <v>60924</v>
       </c>
     </row>
     <row r="97">
@@ -2100,13 +1778,13 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>35338</v>
+        <v>58067</v>
       </c>
       <c r="C97" t="n">
-        <v>44978</v>
+        <v>61886</v>
       </c>
       <c r="D97" t="n">
-        <v>40824.6</v>
+        <v>60343.75</v>
       </c>
     </row>
     <row r="98">
@@ -2114,13 +1792,13 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>39887</v>
+        <v>59557</v>
       </c>
       <c r="C98" t="n">
-        <v>42587</v>
+        <v>61886</v>
       </c>
       <c r="D98" t="n">
-        <v>40651.8</v>
+        <v>61303.75</v>
       </c>
     </row>
     <row r="99">
@@ -2128,13 +1806,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>33831</v>
+        <v>61886</v>
       </c>
       <c r="C99" t="n">
-        <v>42718</v>
+        <v>61886</v>
       </c>
       <c r="D99" t="n">
-        <v>38980.6</v>
+        <v>61886</v>
       </c>
     </row>
     <row r="100">
@@ -2142,13 +1820,13 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>38597</v>
+        <v>61886</v>
       </c>
       <c r="C100" t="n">
-        <v>42625</v>
+        <v>61886</v>
       </c>
       <c r="D100" t="n">
-        <v>41096.2</v>
+        <v>61886</v>
       </c>
     </row>
     <row r="101">
@@ -2156,13 +1834,13 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>37769</v>
+        <v>61837</v>
       </c>
       <c r="C101" t="n">
-        <v>41091</v>
+        <v>61886</v>
       </c>
       <c r="D101" t="n">
-        <v>39457</v>
+        <v>61873.75</v>
       </c>
     </row>
     <row r="102">
@@ -2170,13 +1848,13 @@
         <v>101</v>
       </c>
       <c r="B102" t="n">
-        <v>41527</v>
+        <v>59555</v>
       </c>
       <c r="C102" t="n">
-        <v>43582</v>
+        <v>62254</v>
       </c>
       <c r="D102" t="n">
-        <v>42665.8</v>
+        <v>61395.25</v>
       </c>
     </row>
     <row r="103">
@@ -2184,13 +1862,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="n">
-        <v>36945</v>
+        <v>61886</v>
       </c>
       <c r="C103" t="n">
-        <v>42449</v>
+        <v>62254</v>
       </c>
       <c r="D103" t="n">
-        <v>40116.6</v>
+        <v>62162</v>
       </c>
     </row>
     <row r="104">
@@ -2198,13 +1876,13 @@
         <v>103</v>
       </c>
       <c r="B104" t="n">
-        <v>37924</v>
+        <v>62254</v>
       </c>
       <c r="C104" t="n">
-        <v>44408</v>
+        <v>62254</v>
       </c>
       <c r="D104" t="n">
-        <v>41362.8</v>
+        <v>62254</v>
       </c>
     </row>
     <row r="105">
@@ -2212,13 +1890,13 @@
         <v>104</v>
       </c>
       <c r="B105" t="n">
-        <v>37037</v>
+        <v>62254</v>
       </c>
       <c r="C105" t="n">
-        <v>41977</v>
+        <v>62254</v>
       </c>
       <c r="D105" t="n">
-        <v>39617.2</v>
+        <v>62254</v>
       </c>
     </row>
     <row r="106">
@@ -2226,13 +1904,13 @@
         <v>105</v>
       </c>
       <c r="B106" t="n">
-        <v>35753</v>
+        <v>62254</v>
       </c>
       <c r="C106" t="n">
-        <v>43246</v>
+        <v>62254</v>
       </c>
       <c r="D106" t="n">
-        <v>39475.6</v>
+        <v>62254</v>
       </c>
     </row>
     <row r="107">
@@ -2240,13 +1918,13 @@
         <v>106</v>
       </c>
       <c r="B107" t="n">
-        <v>39602</v>
+        <v>61052</v>
       </c>
       <c r="C107" t="n">
-        <v>44673</v>
+        <v>62254</v>
       </c>
       <c r="D107" t="n">
-        <v>42362.6</v>
+        <v>61953.5</v>
       </c>
     </row>
     <row r="108">
@@ -2254,13 +1932,13 @@
         <v>107</v>
       </c>
       <c r="B108" t="n">
-        <v>39723</v>
+        <v>62254</v>
       </c>
       <c r="C108" t="n">
-        <v>44032</v>
+        <v>62254</v>
       </c>
       <c r="D108" t="n">
-        <v>41727.6</v>
+        <v>62254</v>
       </c>
     </row>
     <row r="109">
@@ -2268,13 +1946,13 @@
         <v>108</v>
       </c>
       <c r="B109" t="n">
-        <v>39241</v>
+        <v>62254</v>
       </c>
       <c r="C109" t="n">
-        <v>43204</v>
+        <v>62254</v>
       </c>
       <c r="D109" t="n">
-        <v>40660.8</v>
+        <v>62254</v>
       </c>
     </row>
     <row r="110">
@@ -2282,13 +1960,13 @@
         <v>109</v>
       </c>
       <c r="B110" t="n">
-        <v>39156</v>
+        <v>62254</v>
       </c>
       <c r="C110" t="n">
-        <v>43017</v>
+        <v>62254</v>
       </c>
       <c r="D110" t="n">
-        <v>41019.6</v>
+        <v>62254</v>
       </c>
     </row>
     <row r="111">
@@ -2296,13 +1974,13 @@
         <v>110</v>
       </c>
       <c r="B111" t="n">
-        <v>36869</v>
+        <v>62254</v>
       </c>
       <c r="C111" t="n">
-        <v>43807</v>
+        <v>62254</v>
       </c>
       <c r="D111" t="n">
-        <v>40332</v>
+        <v>62254</v>
       </c>
     </row>
     <row r="112">
@@ -2310,13 +1988,13 @@
         <v>111</v>
       </c>
       <c r="B112" t="n">
-        <v>38756</v>
+        <v>62254</v>
       </c>
       <c r="C112" t="n">
-        <v>43077</v>
+        <v>62254</v>
       </c>
       <c r="D112" t="n">
-        <v>40938.4</v>
+        <v>62254</v>
       </c>
     </row>
     <row r="113">
@@ -2324,13 +2002,13 @@
         <v>112</v>
       </c>
       <c r="B113" t="n">
-        <v>38128</v>
+        <v>61176</v>
       </c>
       <c r="C113" t="n">
-        <v>42291</v>
+        <v>62254</v>
       </c>
       <c r="D113" t="n">
-        <v>39887.2</v>
+        <v>61944</v>
       </c>
     </row>
     <row r="114">
@@ -2338,13 +2016,13 @@
         <v>113</v>
       </c>
       <c r="B114" t="n">
-        <v>37653</v>
+        <v>60983</v>
       </c>
       <c r="C114" t="n">
-        <v>42821</v>
+        <v>62254</v>
       </c>
       <c r="D114" t="n">
-        <v>40860.8</v>
+        <v>61936.25</v>
       </c>
     </row>
     <row r="115">
@@ -2352,13 +2030,13 @@
         <v>114</v>
       </c>
       <c r="B115" t="n">
-        <v>33669</v>
+        <v>60983</v>
       </c>
       <c r="C115" t="n">
-        <v>44092</v>
+        <v>62254</v>
       </c>
       <c r="D115" t="n">
-        <v>40710.8</v>
+        <v>61936.25</v>
       </c>
     </row>
     <row r="116">
@@ -2366,13 +2044,13 @@
         <v>115</v>
       </c>
       <c r="B116" t="n">
-        <v>38944</v>
+        <v>62254</v>
       </c>
       <c r="C116" t="n">
-        <v>42750</v>
+        <v>62254</v>
       </c>
       <c r="D116" t="n">
-        <v>40656.8</v>
+        <v>62254</v>
       </c>
     </row>
     <row r="117">
@@ -2380,13 +2058,13 @@
         <v>116</v>
       </c>
       <c r="B117" t="n">
-        <v>41741</v>
+        <v>62254</v>
       </c>
       <c r="C117" t="n">
-        <v>43197</v>
+        <v>62254</v>
       </c>
       <c r="D117" t="n">
-        <v>42477</v>
+        <v>62254</v>
       </c>
     </row>
     <row r="118">
@@ -2394,13 +2072,13 @@
         <v>117</v>
       </c>
       <c r="B118" t="n">
-        <v>38238</v>
+        <v>62254</v>
       </c>
       <c r="C118" t="n">
-        <v>44978</v>
+        <v>62325</v>
       </c>
       <c r="D118" t="n">
-        <v>41522.6</v>
+        <v>62271.75</v>
       </c>
     </row>
     <row r="119">
@@ -2408,13 +2086,13 @@
         <v>118</v>
       </c>
       <c r="B119" t="n">
-        <v>39025</v>
+        <v>62254</v>
       </c>
       <c r="C119" t="n">
-        <v>43493</v>
+        <v>62325</v>
       </c>
       <c r="D119" t="n">
-        <v>40645</v>
+        <v>62271.75</v>
       </c>
     </row>
     <row r="120">
@@ -2422,13 +2100,13 @@
         <v>119</v>
       </c>
       <c r="B120" t="n">
-        <v>34594</v>
+        <v>60680</v>
       </c>
       <c r="C120" t="n">
-        <v>44477</v>
+        <v>63298</v>
       </c>
       <c r="D120" t="n">
-        <v>39727.4</v>
+        <v>62157</v>
       </c>
     </row>
     <row r="121">
@@ -2436,13 +2114,13 @@
         <v>120</v>
       </c>
       <c r="B121" t="n">
-        <v>39076</v>
+        <v>62325</v>
       </c>
       <c r="C121" t="n">
-        <v>43411</v>
+        <v>63298</v>
       </c>
       <c r="D121" t="n">
-        <v>41318</v>
+        <v>63054.75</v>
       </c>
     </row>
     <row r="122">
@@ -2450,13 +2128,13 @@
         <v>121</v>
       </c>
       <c r="B122" t="n">
-        <v>39061</v>
+        <v>62793</v>
       </c>
       <c r="C122" t="n">
-        <v>43814</v>
+        <v>63298</v>
       </c>
       <c r="D122" t="n">
-        <v>40934.4</v>
+        <v>63171.75</v>
       </c>
     </row>
     <row r="123">
@@ -2464,13 +2142,13 @@
         <v>122</v>
       </c>
       <c r="B123" t="n">
-        <v>38153</v>
+        <v>62793</v>
       </c>
       <c r="C123" t="n">
-        <v>43471</v>
+        <v>63298</v>
       </c>
       <c r="D123" t="n">
-        <v>40314.2</v>
+        <v>63090</v>
       </c>
     </row>
     <row r="124">
@@ -2478,13 +2156,13 @@
         <v>123</v>
       </c>
       <c r="B124" t="n">
-        <v>38444</v>
+        <v>61826</v>
       </c>
       <c r="C124" t="n">
-        <v>43215</v>
+        <v>63298</v>
       </c>
       <c r="D124" t="n">
-        <v>41330</v>
+        <v>62567</v>
       </c>
     </row>
     <row r="125">
@@ -2492,13 +2170,13 @@
         <v>124</v>
       </c>
       <c r="B125" t="n">
-        <v>38323</v>
+        <v>61221</v>
       </c>
       <c r="C125" t="n">
-        <v>44052</v>
+        <v>61846</v>
       </c>
       <c r="D125" t="n">
-        <v>41883.4</v>
+        <v>61545.5</v>
       </c>
     </row>
     <row r="126">
@@ -2506,13 +2184,13 @@
         <v>125</v>
       </c>
       <c r="B126" t="n">
-        <v>36885</v>
+        <v>59752</v>
       </c>
       <c r="C126" t="n">
-        <v>40777</v>
+        <v>63586</v>
       </c>
       <c r="D126" t="n">
-        <v>38284</v>
+        <v>61449</v>
       </c>
     </row>
     <row r="127">
@@ -2520,13 +2198,13 @@
         <v>126</v>
       </c>
       <c r="B127" t="n">
-        <v>39608</v>
+        <v>59261</v>
       </c>
       <c r="C127" t="n">
-        <v>44052</v>
+        <v>63586</v>
       </c>
       <c r="D127" t="n">
-        <v>42092</v>
+        <v>60980.25</v>
       </c>
     </row>
     <row r="128">
@@ -2534,13 +2212,13 @@
         <v>127</v>
       </c>
       <c r="B128" t="n">
-        <v>38128</v>
+        <v>60537</v>
       </c>
       <c r="C128" t="n">
-        <v>44152</v>
+        <v>64628</v>
       </c>
       <c r="D128" t="n">
-        <v>40831</v>
+        <v>62322</v>
       </c>
     </row>
     <row r="129">
@@ -2548,13 +2226,13 @@
         <v>128</v>
       </c>
       <c r="B129" t="n">
-        <v>37148</v>
+        <v>60588</v>
       </c>
       <c r="C129" t="n">
-        <v>43431</v>
+        <v>63586</v>
       </c>
       <c r="D129" t="n">
-        <v>40330</v>
+        <v>62678.75</v>
       </c>
     </row>
     <row r="130">
@@ -2562,13 +2240,13 @@
         <v>129</v>
       </c>
       <c r="B130" t="n">
-        <v>39595</v>
+        <v>62361</v>
       </c>
       <c r="C130" t="n">
-        <v>43981</v>
+        <v>64358</v>
       </c>
       <c r="D130" t="n">
-        <v>41714.4</v>
+        <v>63158.5</v>
       </c>
     </row>
     <row r="131">
@@ -2576,13 +2254,13 @@
         <v>130</v>
       </c>
       <c r="B131" t="n">
-        <v>39442</v>
+        <v>62070</v>
       </c>
       <c r="C131" t="n">
-        <v>41396</v>
+        <v>63681</v>
       </c>
       <c r="D131" t="n">
-        <v>40167.2</v>
+        <v>62614.75</v>
       </c>
     </row>
     <row r="132">
@@ -2590,13 +2268,13 @@
         <v>131</v>
       </c>
       <c r="B132" t="n">
-        <v>36422</v>
+        <v>60729</v>
       </c>
       <c r="C132" t="n">
-        <v>42302</v>
+        <v>62505</v>
       </c>
       <c r="D132" t="n">
-        <v>39424.4</v>
+        <v>62061</v>
       </c>
     </row>
     <row r="133">
@@ -2604,13 +2282,13 @@
         <v>132</v>
       </c>
       <c r="B133" t="n">
-        <v>39028</v>
+        <v>60351</v>
       </c>
       <c r="C133" t="n">
-        <v>44406</v>
+        <v>63700</v>
       </c>
       <c r="D133" t="n">
-        <v>41672.2</v>
+        <v>62265.25</v>
       </c>
     </row>
     <row r="134">
@@ -2618,13 +2296,13 @@
         <v>133</v>
       </c>
       <c r="B134" t="n">
-        <v>35819</v>
+        <v>62505</v>
       </c>
       <c r="C134" t="n">
-        <v>43758</v>
+        <v>63700</v>
       </c>
       <c r="D134" t="n">
-        <v>39826.8</v>
+        <v>63238</v>
       </c>
     </row>
     <row r="135">
@@ -2632,13 +2310,13 @@
         <v>134</v>
       </c>
       <c r="B135" t="n">
-        <v>39753</v>
+        <v>58784</v>
       </c>
       <c r="C135" t="n">
-        <v>44092</v>
+        <v>63700</v>
       </c>
       <c r="D135" t="n">
-        <v>41472.2</v>
+        <v>62258.75</v>
       </c>
     </row>
     <row r="136">
@@ -2646,13 +2324,13 @@
         <v>135</v>
       </c>
       <c r="B136" t="n">
-        <v>35914</v>
+        <v>62851</v>
       </c>
       <c r="C136" t="n">
-        <v>43166</v>
+        <v>63700</v>
       </c>
       <c r="D136" t="n">
-        <v>41117.6</v>
+        <v>63487.75</v>
       </c>
     </row>
     <row r="137">
@@ -2660,13 +2338,13 @@
         <v>136</v>
       </c>
       <c r="B137" t="n">
-        <v>38029</v>
+        <v>61696</v>
       </c>
       <c r="C137" t="n">
-        <v>42585</v>
+        <v>63700</v>
       </c>
       <c r="D137" t="n">
-        <v>39993</v>
+        <v>62723.25</v>
       </c>
     </row>
     <row r="138">
@@ -2674,13 +2352,13 @@
         <v>137</v>
       </c>
       <c r="B138" t="n">
-        <v>38963</v>
+        <v>63008</v>
       </c>
       <c r="C138" t="n">
-        <v>43825</v>
+        <v>63700</v>
       </c>
       <c r="D138" t="n">
-        <v>40966.8</v>
+        <v>63527</v>
       </c>
     </row>
     <row r="139">
@@ -2688,13 +2366,13 @@
         <v>138</v>
       </c>
       <c r="B139" t="n">
-        <v>41171</v>
+        <v>59946</v>
       </c>
       <c r="C139" t="n">
-        <v>43413</v>
+        <v>61474</v>
       </c>
       <c r="D139" t="n">
-        <v>41952</v>
+        <v>60691.5</v>
       </c>
     </row>
     <row r="140">
@@ -2702,13 +2380,13 @@
         <v>139</v>
       </c>
       <c r="B140" t="n">
-        <v>41552</v>
+        <v>60701</v>
       </c>
       <c r="C140" t="n">
-        <v>43805</v>
+        <v>61400</v>
       </c>
       <c r="D140" t="n">
-        <v>42823.6</v>
+        <v>61157.5</v>
       </c>
     </row>
     <row r="141">
@@ -2716,13 +2394,13 @@
         <v>140</v>
       </c>
       <c r="B141" t="n">
-        <v>39928</v>
+        <v>60701</v>
       </c>
       <c r="C141" t="n">
-        <v>42636</v>
+        <v>63700</v>
       </c>
       <c r="D141" t="n">
-        <v>41395</v>
+        <v>62116</v>
       </c>
     </row>
     <row r="142">
@@ -2730,13 +2408,13 @@
         <v>141</v>
       </c>
       <c r="B142" t="n">
-        <v>39093</v>
+        <v>60949</v>
       </c>
       <c r="C142" t="n">
-        <v>41621</v>
+        <v>62663</v>
       </c>
       <c r="D142" t="n">
-        <v>40247.6</v>
+        <v>61830.5</v>
       </c>
     </row>
     <row r="143">
@@ -2744,13 +2422,13 @@
         <v>142</v>
       </c>
       <c r="B143" t="n">
-        <v>41405</v>
+        <v>61047</v>
       </c>
       <c r="C143" t="n">
-        <v>44210</v>
+        <v>62687</v>
       </c>
       <c r="D143" t="n">
-        <v>42625.8</v>
+        <v>61861</v>
       </c>
     </row>
     <row r="144">
@@ -2758,13 +2436,13 @@
         <v>143</v>
       </c>
       <c r="B144" t="n">
-        <v>40002</v>
+        <v>61047</v>
       </c>
       <c r="C144" t="n">
-        <v>44052</v>
+        <v>62663</v>
       </c>
       <c r="D144" t="n">
-        <v>41965.4</v>
+        <v>61998</v>
       </c>
     </row>
     <row r="145">
@@ -2772,13 +2450,13 @@
         <v>144</v>
       </c>
       <c r="B145" t="n">
-        <v>39757</v>
+        <v>61853</v>
       </c>
       <c r="C145" t="n">
-        <v>44052</v>
+        <v>62663</v>
       </c>
       <c r="D145" t="n">
-        <v>40943</v>
+        <v>62199.5</v>
       </c>
     </row>
     <row r="146">
@@ -2786,13 +2464,13 @@
         <v>145</v>
       </c>
       <c r="B146" t="n">
-        <v>36021</v>
+        <v>60113</v>
       </c>
       <c r="C146" t="n">
-        <v>42832</v>
+        <v>62429</v>
       </c>
       <c r="D146" t="n">
-        <v>40594.8</v>
+        <v>61550.25</v>
       </c>
     </row>
     <row r="147">
@@ -2800,13 +2478,13 @@
         <v>146</v>
       </c>
       <c r="B147" t="n">
-        <v>38555</v>
+        <v>61853</v>
       </c>
       <c r="C147" t="n">
-        <v>43571</v>
+        <v>62429</v>
       </c>
       <c r="D147" t="n">
-        <v>40888.4</v>
+        <v>62206</v>
       </c>
     </row>
     <row r="148">
@@ -2814,13 +2492,13 @@
         <v>147</v>
       </c>
       <c r="B148" t="n">
-        <v>39014</v>
+        <v>60377</v>
       </c>
       <c r="C148" t="n">
-        <v>41946</v>
+        <v>62500</v>
       </c>
       <c r="D148" t="n">
-        <v>40691.6</v>
+        <v>61832.75</v>
       </c>
     </row>
     <row r="149">
@@ -2828,13 +2506,13 @@
         <v>148</v>
       </c>
       <c r="B149" t="n">
-        <v>39196</v>
+        <v>57649</v>
       </c>
       <c r="C149" t="n">
-        <v>40926</v>
+        <v>62500</v>
       </c>
       <c r="D149" t="n">
-        <v>40279.4</v>
+        <v>61142</v>
       </c>
     </row>
     <row r="150">
@@ -2842,13 +2520,13 @@
         <v>149</v>
       </c>
       <c r="B150" t="n">
-        <v>39165</v>
+        <v>61919</v>
       </c>
       <c r="C150" t="n">
-        <v>44918</v>
+        <v>62500</v>
       </c>
       <c r="D150" t="n">
-        <v>41977.4</v>
+        <v>62354.75</v>
       </c>
     </row>
     <row r="151">
@@ -2856,13 +2534,13 @@
         <v>150</v>
       </c>
       <c r="B151" t="n">
-        <v>40428</v>
+        <v>62500</v>
       </c>
       <c r="C151" t="n">
-        <v>44733</v>
+        <v>62500</v>
       </c>
       <c r="D151" t="n">
-        <v>42637.4</v>
+        <v>62500</v>
       </c>
     </row>
     <row r="152">
@@ -2870,13 +2548,13 @@
         <v>151</v>
       </c>
       <c r="B152" t="n">
-        <v>37022</v>
+        <v>62500</v>
       </c>
       <c r="C152" t="n">
-        <v>43502</v>
+        <v>62500</v>
       </c>
       <c r="D152" t="n">
-        <v>40604.8</v>
+        <v>62500</v>
       </c>
     </row>
     <row r="153">
@@ -2884,13 +2562,13 @@
         <v>152</v>
       </c>
       <c r="B153" t="n">
-        <v>36796</v>
+        <v>61062</v>
       </c>
       <c r="C153" t="n">
-        <v>40461</v>
+        <v>62500</v>
       </c>
       <c r="D153" t="n">
-        <v>38968</v>
+        <v>62140.5</v>
       </c>
     </row>
     <row r="154">
@@ -2898,13 +2576,13 @@
         <v>153</v>
       </c>
       <c r="B154" t="n">
-        <v>38684</v>
+        <v>60239</v>
       </c>
       <c r="C154" t="n">
-        <v>42821</v>
+        <v>62500</v>
       </c>
       <c r="D154" t="n">
-        <v>40833.2</v>
+        <v>61881.25</v>
       </c>
     </row>
     <row r="155">
@@ -2912,13 +2590,13 @@
         <v>154</v>
       </c>
       <c r="B155" t="n">
-        <v>39490</v>
+        <v>60363</v>
       </c>
       <c r="C155" t="n">
-        <v>44564</v>
+        <v>62500</v>
       </c>
       <c r="D155" t="n">
-        <v>42063.8</v>
+        <v>61609</v>
       </c>
     </row>
     <row r="156">
@@ -2926,13 +2604,13 @@
         <v>155</v>
       </c>
       <c r="B156" t="n">
-        <v>38168</v>
+        <v>59362</v>
       </c>
       <c r="C156" t="n">
-        <v>41861</v>
+        <v>62500</v>
       </c>
       <c r="D156" t="n">
-        <v>39728</v>
+        <v>61024.25</v>
       </c>
     </row>
     <row r="157">
@@ -2940,13 +2618,13 @@
         <v>156</v>
       </c>
       <c r="B157" t="n">
-        <v>37700</v>
+        <v>59436</v>
       </c>
       <c r="C157" t="n">
-        <v>43551</v>
+        <v>62500</v>
       </c>
       <c r="D157" t="n">
-        <v>41328.6</v>
+        <v>60472.5</v>
       </c>
     </row>
     <row r="158">
@@ -2954,13 +2632,13 @@
         <v>157</v>
       </c>
       <c r="B158" t="n">
-        <v>36433</v>
+        <v>56971</v>
       </c>
       <c r="C158" t="n">
-        <v>43473</v>
+        <v>60219</v>
       </c>
       <c r="D158" t="n">
-        <v>40059.8</v>
+        <v>58999</v>
       </c>
     </row>
     <row r="159">
@@ -2968,13 +2646,13 @@
         <v>158</v>
       </c>
       <c r="B159" t="n">
-        <v>39648</v>
+        <v>59515</v>
       </c>
       <c r="C159" t="n">
-        <v>44081</v>
+        <v>61198</v>
       </c>
       <c r="D159" t="n">
-        <v>41769.2</v>
+        <v>60287.75</v>
       </c>
     </row>
     <row r="160">
@@ -2982,13 +2660,13 @@
         <v>159</v>
       </c>
       <c r="B160" t="n">
-        <v>39931</v>
+        <v>58767</v>
       </c>
       <c r="C160" t="n">
-        <v>42467</v>
+        <v>61198</v>
       </c>
       <c r="D160" t="n">
-        <v>41039.8</v>
+        <v>59839.5</v>
       </c>
     </row>
     <row r="161">
@@ -2996,13 +2674,13 @@
         <v>160</v>
       </c>
       <c r="B161" t="n">
-        <v>36879</v>
+        <v>57185</v>
       </c>
       <c r="C161" t="n">
-        <v>41668</v>
+        <v>61198</v>
       </c>
       <c r="D161" t="n">
-        <v>40038</v>
+        <v>59950</v>
       </c>
     </row>
     <row r="162">
@@ -3010,13 +2688,13 @@
         <v>161</v>
       </c>
       <c r="B162" t="n">
-        <v>35864</v>
+        <v>60733</v>
       </c>
       <c r="C162" t="n">
-        <v>42440</v>
+        <v>61198</v>
       </c>
       <c r="D162" t="n">
-        <v>40397.8</v>
+        <v>61081.75</v>
       </c>
     </row>
     <row r="163">
@@ -3024,13 +2702,13 @@
         <v>162</v>
       </c>
       <c r="B163" t="n">
-        <v>39197</v>
+        <v>61198</v>
       </c>
       <c r="C163" t="n">
-        <v>43382</v>
+        <v>61198</v>
       </c>
       <c r="D163" t="n">
-        <v>41888.2</v>
+        <v>61198</v>
       </c>
     </row>
     <row r="164">
@@ -3038,13 +2716,13 @@
         <v>163</v>
       </c>
       <c r="B164" t="n">
-        <v>38854</v>
+        <v>61198</v>
       </c>
       <c r="C164" t="n">
-        <v>41338</v>
+        <v>61198</v>
       </c>
       <c r="D164" t="n">
-        <v>40453</v>
+        <v>61198</v>
       </c>
     </row>
     <row r="165">
@@ -3052,13 +2730,13 @@
         <v>164</v>
       </c>
       <c r="B165" t="n">
-        <v>41042</v>
+        <v>57315</v>
       </c>
       <c r="C165" t="n">
-        <v>44386</v>
+        <v>61198</v>
       </c>
       <c r="D165" t="n">
-        <v>42798.2</v>
+        <v>59471</v>
       </c>
     </row>
     <row r="166">
@@ -3066,13 +2744,13 @@
         <v>165</v>
       </c>
       <c r="B166" t="n">
-        <v>38971</v>
+        <v>61108</v>
       </c>
       <c r="C166" t="n">
-        <v>43747</v>
+        <v>61198</v>
       </c>
       <c r="D166" t="n">
-        <v>41479</v>
+        <v>61153</v>
       </c>
     </row>
     <row r="167">
@@ -3080,13 +2758,13 @@
         <v>166</v>
       </c>
       <c r="B167" t="n">
-        <v>38457</v>
+        <v>60643</v>
       </c>
       <c r="C167" t="n">
-        <v>44326</v>
+        <v>61198</v>
       </c>
       <c r="D167" t="n">
-        <v>41404</v>
+        <v>60905</v>
       </c>
     </row>
     <row r="168">
@@ -3094,13 +2772,13 @@
         <v>167</v>
       </c>
       <c r="B168" t="n">
-        <v>36954</v>
+        <v>59212</v>
       </c>
       <c r="C168" t="n">
-        <v>44733</v>
+        <v>61198</v>
       </c>
       <c r="D168" t="n">
-        <v>40644.4</v>
+        <v>60615.5</v>
       </c>
     </row>
     <row r="169">
@@ -3108,13 +2786,13 @@
         <v>168</v>
       </c>
       <c r="B169" t="n">
-        <v>40486</v>
+        <v>59747</v>
       </c>
       <c r="C169" t="n">
-        <v>43698</v>
+        <v>61406</v>
       </c>
       <c r="D169" t="n">
-        <v>41929.4</v>
+        <v>60643.25</v>
       </c>
     </row>
     <row r="170">
@@ -3122,13 +2800,13 @@
         <v>169</v>
       </c>
       <c r="B170" t="n">
-        <v>38102</v>
+        <v>58934</v>
       </c>
       <c r="C170" t="n">
-        <v>43696</v>
+        <v>61406</v>
       </c>
       <c r="D170" t="n">
-        <v>40534.2</v>
+        <v>60477.5</v>
       </c>
     </row>
     <row r="171">
@@ -3136,13 +2814,13 @@
         <v>170</v>
       </c>
       <c r="B171" t="n">
-        <v>37616</v>
+        <v>57552</v>
       </c>
       <c r="C171" t="n">
-        <v>44711</v>
+        <v>62924</v>
       </c>
       <c r="D171" t="n">
-        <v>41244</v>
+        <v>60519.75</v>
       </c>
     </row>
     <row r="172">
@@ -3150,13 +2828,13 @@
         <v>171</v>
       </c>
       <c r="B172" t="n">
-        <v>41338</v>
+        <v>58492</v>
       </c>
       <c r="C172" t="n">
-        <v>42872</v>
+        <v>63176</v>
       </c>
       <c r="D172" t="n">
-        <v>41836.2</v>
+        <v>60817.75</v>
       </c>
     </row>
     <row r="173">
@@ -3164,13 +2842,13 @@
         <v>172</v>
       </c>
       <c r="B173" t="n">
-        <v>36440</v>
+        <v>59972</v>
       </c>
       <c r="C173" t="n">
-        <v>43435</v>
+        <v>63176</v>
       </c>
       <c r="D173" t="n">
-        <v>40183.8</v>
+        <v>61711.75</v>
       </c>
     </row>
     <row r="174">
@@ -3178,13 +2856,13 @@
         <v>173</v>
       </c>
       <c r="B174" t="n">
-        <v>39513</v>
+        <v>58068</v>
       </c>
       <c r="C174" t="n">
-        <v>43511</v>
+        <v>63176</v>
       </c>
       <c r="D174" t="n">
-        <v>41766.2</v>
+        <v>61234.5</v>
       </c>
     </row>
     <row r="175">
@@ -3192,13 +2870,13 @@
         <v>174</v>
       </c>
       <c r="B175" t="n">
-        <v>38893</v>
+        <v>60087</v>
       </c>
       <c r="C175" t="n">
-        <v>40256</v>
+        <v>63176</v>
       </c>
       <c r="D175" t="n">
-        <v>39585</v>
+        <v>61879.5</v>
       </c>
     </row>
     <row r="176">
@@ -3206,13 +2884,13 @@
         <v>175</v>
       </c>
       <c r="B176" t="n">
-        <v>36853</v>
+        <v>60151</v>
       </c>
       <c r="C176" t="n">
-        <v>42362</v>
+        <v>63176</v>
       </c>
       <c r="D176" t="n">
-        <v>40035.4</v>
+        <v>62335.75</v>
       </c>
     </row>
     <row r="177">
@@ -3220,13 +2898,13 @@
         <v>176</v>
       </c>
       <c r="B177" t="n">
-        <v>39808</v>
+        <v>61851</v>
       </c>
       <c r="C177" t="n">
-        <v>44477</v>
+        <v>63176</v>
       </c>
       <c r="D177" t="n">
-        <v>42962.2</v>
+        <v>62539.75</v>
       </c>
     </row>
     <row r="178">
@@ -3234,13 +2912,13 @@
         <v>177</v>
       </c>
       <c r="B178" t="n">
-        <v>38473</v>
+        <v>61851</v>
       </c>
       <c r="C178" t="n">
-        <v>42077</v>
+        <v>63176</v>
       </c>
       <c r="D178" t="n">
-        <v>40548.2</v>
+        <v>62539.75</v>
       </c>
     </row>
     <row r="179">
@@ -3248,13 +2926,13 @@
         <v>178</v>
       </c>
       <c r="B179" t="n">
-        <v>35473</v>
+        <v>56033</v>
       </c>
       <c r="C179" t="n">
-        <v>44662</v>
+        <v>63247</v>
       </c>
       <c r="D179" t="n">
-        <v>40503.6</v>
+        <v>61255.5</v>
       </c>
     </row>
     <row r="180">
@@ -3262,13 +2940,13 @@
         <v>179</v>
       </c>
       <c r="B180" t="n">
-        <v>38282</v>
+        <v>63247</v>
       </c>
       <c r="C180" t="n">
-        <v>42888</v>
+        <v>63247</v>
       </c>
       <c r="D180" t="n">
-        <v>40631.8</v>
+        <v>63247</v>
       </c>
     </row>
     <row r="181">
@@ -3276,13 +2954,13 @@
         <v>180</v>
       </c>
       <c r="B181" t="n">
-        <v>40122</v>
+        <v>63247</v>
       </c>
       <c r="C181" t="n">
-        <v>43471</v>
+        <v>63247</v>
       </c>
       <c r="D181" t="n">
-        <v>41633.4</v>
+        <v>63247</v>
       </c>
     </row>
     <row r="182">
@@ -3290,13 +2968,13 @@
         <v>181</v>
       </c>
       <c r="B182" t="n">
-        <v>38536</v>
+        <v>63247</v>
       </c>
       <c r="C182" t="n">
-        <v>44869</v>
+        <v>63247</v>
       </c>
       <c r="D182" t="n">
-        <v>42194.2</v>
+        <v>63247</v>
       </c>
     </row>
     <row r="183">
@@ -3304,13 +2982,13 @@
         <v>182</v>
       </c>
       <c r="B183" t="n">
-        <v>37588</v>
+        <v>63247</v>
       </c>
       <c r="C183" t="n">
-        <v>43551</v>
+        <v>63247</v>
       </c>
       <c r="D183" t="n">
-        <v>40437.8</v>
+        <v>63247</v>
       </c>
     </row>
     <row r="184">
@@ -3318,13 +2996,13 @@
         <v>183</v>
       </c>
       <c r="B184" t="n">
-        <v>36921</v>
+        <v>61723</v>
       </c>
       <c r="C184" t="n">
-        <v>43257</v>
+        <v>63247</v>
       </c>
       <c r="D184" t="n">
-        <v>40955.6</v>
+        <v>62815.25</v>
       </c>
     </row>
     <row r="185">
@@ -3332,13 +3010,13 @@
         <v>184</v>
       </c>
       <c r="B185" t="n">
-        <v>38266</v>
+        <v>61825</v>
       </c>
       <c r="C185" t="n">
-        <v>43502</v>
+        <v>63466</v>
       </c>
       <c r="D185" t="n">
-        <v>41309</v>
+        <v>62726.25</v>
       </c>
     </row>
     <row r="186">
@@ -3346,13 +3024,13 @@
         <v>185</v>
       </c>
       <c r="B186" t="n">
-        <v>40049</v>
+        <v>60628</v>
       </c>
       <c r="C186" t="n">
-        <v>44003</v>
+        <v>63466</v>
       </c>
       <c r="D186" t="n">
-        <v>42455.6</v>
+        <v>62433.75</v>
       </c>
     </row>
     <row r="187">
@@ -3360,13 +3038,13 @@
         <v>186</v>
       </c>
       <c r="B187" t="n">
-        <v>37687</v>
+        <v>63075</v>
       </c>
       <c r="C187" t="n">
-        <v>42046</v>
+        <v>64494</v>
       </c>
       <c r="D187" t="n">
-        <v>40367.4</v>
+        <v>63614</v>
       </c>
     </row>
     <row r="188">
@@ -3374,13 +3052,13 @@
         <v>187</v>
       </c>
       <c r="B188" t="n">
-        <v>39310</v>
+        <v>62764</v>
       </c>
       <c r="C188" t="n">
-        <v>42761</v>
+        <v>64494</v>
       </c>
       <c r="D188" t="n">
-        <v>41163.4</v>
+        <v>63542</v>
       </c>
     </row>
     <row r="189">
@@ -3388,13 +3066,13 @@
         <v>188</v>
       </c>
       <c r="B189" t="n">
-        <v>34787</v>
+        <v>62886</v>
       </c>
       <c r="C189" t="n">
-        <v>42576</v>
+        <v>64494</v>
       </c>
       <c r="D189" t="n">
-        <v>39207.8</v>
+        <v>63578.5</v>
       </c>
     </row>
     <row r="190">
@@ -3402,13 +3080,13 @@
         <v>189</v>
       </c>
       <c r="B190" t="n">
-        <v>40583</v>
+        <v>63490</v>
       </c>
       <c r="C190" t="n">
-        <v>43435</v>
+        <v>64494</v>
       </c>
       <c r="D190" t="n">
-        <v>41963.4</v>
+        <v>63992</v>
       </c>
     </row>
     <row r="191">
@@ -3416,13 +3094,13 @@
         <v>190</v>
       </c>
       <c r="B191" t="n">
-        <v>38058</v>
+        <v>61520</v>
       </c>
       <c r="C191" t="n">
-        <v>42921</v>
+        <v>64664</v>
       </c>
       <c r="D191" t="n">
-        <v>39956.4</v>
+        <v>63544</v>
       </c>
     </row>
     <row r="192">
@@ -3430,13 +3108,13 @@
         <v>191</v>
       </c>
       <c r="B192" t="n">
-        <v>36939</v>
+        <v>61793</v>
       </c>
       <c r="C192" t="n">
-        <v>43186</v>
+        <v>64436</v>
       </c>
       <c r="D192" t="n">
-        <v>40824.2</v>
+        <v>63335.25</v>
       </c>
     </row>
     <row r="193">
@@ -3444,13 +3122,13 @@
         <v>192</v>
       </c>
       <c r="B193" t="n">
-        <v>39415</v>
+        <v>63556</v>
       </c>
       <c r="C193" t="n">
-        <v>43540</v>
+        <v>64436</v>
       </c>
       <c r="D193" t="n">
-        <v>41499.8</v>
+        <v>63776</v>
       </c>
     </row>
     <row r="194">
@@ -3458,13 +3136,13 @@
         <v>193</v>
       </c>
       <c r="B194" t="n">
-        <v>36157</v>
+        <v>62752</v>
       </c>
       <c r="C194" t="n">
-        <v>42271</v>
+        <v>63910</v>
       </c>
       <c r="D194" t="n">
-        <v>39006.8</v>
+        <v>63372</v>
       </c>
     </row>
     <row r="195">
@@ -3472,13 +3150,13 @@
         <v>194</v>
       </c>
       <c r="B195" t="n">
-        <v>38782</v>
+        <v>63574</v>
       </c>
       <c r="C195" t="n">
-        <v>42558</v>
+        <v>63910</v>
       </c>
       <c r="D195" t="n">
-        <v>40065.8</v>
+        <v>63742</v>
       </c>
     </row>
     <row r="196">
@@ -3486,13 +3164,13 @@
         <v>195</v>
       </c>
       <c r="B196" t="n">
-        <v>36413</v>
+        <v>63574</v>
       </c>
       <c r="C196" t="n">
-        <v>42778</v>
+        <v>63910</v>
       </c>
       <c r="D196" t="n">
-        <v>39451.6</v>
+        <v>63742</v>
       </c>
     </row>
     <row r="197">
@@ -3500,13 +3178,13 @@
         <v>196</v>
       </c>
       <c r="B197" t="n">
-        <v>37992</v>
+        <v>63910</v>
       </c>
       <c r="C197" t="n">
-        <v>44368</v>
+        <v>63910</v>
       </c>
       <c r="D197" t="n">
-        <v>41225.4</v>
+        <v>63910</v>
       </c>
     </row>
     <row r="198">
@@ -3514,13 +3192,13 @@
         <v>197</v>
       </c>
       <c r="B198" t="n">
-        <v>36203</v>
+        <v>62570</v>
       </c>
       <c r="C198" t="n">
-        <v>44348</v>
+        <v>63910</v>
       </c>
       <c r="D198" t="n">
-        <v>41780</v>
+        <v>63376.25</v>
       </c>
     </row>
     <row r="199">
@@ -3528,13 +3206,13 @@
         <v>198</v>
       </c>
       <c r="B199" t="n">
-        <v>36423</v>
+        <v>63190</v>
       </c>
       <c r="C199" t="n">
-        <v>44299</v>
+        <v>63910</v>
       </c>
       <c r="D199" t="n">
-        <v>41048.8</v>
+        <v>63585</v>
       </c>
     </row>
     <row r="200">
@@ -3542,13 +3220,13 @@
         <v>199</v>
       </c>
       <c r="B200" t="n">
-        <v>36047</v>
+        <v>63910</v>
       </c>
       <c r="C200" t="n">
-        <v>44918</v>
+        <v>63910</v>
       </c>
       <c r="D200" t="n">
-        <v>41515.6</v>
+        <v>63910</v>
       </c>
     </row>
     <row r="201">
@@ -3556,13 +3234,13 @@
         <v>200</v>
       </c>
       <c r="B201" t="n">
-        <v>37228</v>
+        <v>60158</v>
       </c>
       <c r="C201" t="n">
-        <v>44074</v>
+        <v>63910</v>
       </c>
       <c r="D201" t="n">
-        <v>40805.4</v>
+        <v>62034</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en los formatos de la salida de valores
</commit_message>
<xml_diff>
--- a/Trabajo Practico Integrador/Salidas/Datos.xlsx
+++ b/Trabajo Practico Integrador/Salidas/Datos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,285 +442,1260 @@
           <t>Media Func. Objetivo</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Potencia total</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>36398</v>
-      </c>
-      <c r="C2" t="n">
-        <v>44733</v>
-      </c>
-      <c r="D2" t="n">
-        <v>40692.28</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>36,581.00</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>44,662.00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>41,460.10</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2,073,005.00</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
-        <v>31779</v>
-      </c>
-      <c r="C3" t="n">
-        <v>47802</v>
-      </c>
-      <c r="D3" t="n">
-        <v>40837.72</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>30,199.00</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>50,983.00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>41,525.00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2,076,250.00</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>30747</v>
-      </c>
-      <c r="C4" t="n">
-        <v>49897</v>
-      </c>
-      <c r="D4" t="n">
-        <v>41035.62</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>33,128.00</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>50,983.00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>42,211.44</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2,110,572.00</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
-        <v>25347</v>
-      </c>
-      <c r="C5" t="n">
-        <v>51482</v>
-      </c>
-      <c r="D5" t="n">
-        <v>40809.56</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>33,263.00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>54,124.00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>42,714.00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2,135,700.00</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
-        <v>27207</v>
-      </c>
-      <c r="C6" t="n">
-        <v>57620</v>
-      </c>
-      <c r="D6" t="n">
-        <v>41428.58</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>33,873.00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>54,124.00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>44,680.64</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2,234,032.00</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
-        <v>30176</v>
-      </c>
-      <c r="C7" t="n">
-        <v>57620</v>
-      </c>
-      <c r="D7" t="n">
-        <v>41524.08</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>33,873.00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>56,689.00</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>45,707.74</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2,285,387.00</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
-        <v>34189</v>
-      </c>
-      <c r="C8" t="n">
-        <v>57620</v>
-      </c>
-      <c r="D8" t="n">
-        <v>43366.96</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>32,947.00</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>56,689.00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>45,187.34</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2,259,367.00</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
-        <v>29674</v>
-      </c>
-      <c r="C9" t="n">
-        <v>57265</v>
-      </c>
-      <c r="D9" t="n">
-        <v>43584.24</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>30,588.00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>58,349.00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>46,756.64</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2,337,832.00</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
-        <v>30589</v>
-      </c>
-      <c r="C10" t="n">
-        <v>56931</v>
-      </c>
-      <c r="D10" t="n">
-        <v>44975.98</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>39,419.00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>58,349.00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>48,273.76</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2,413,688.00</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
-        <v>31918</v>
-      </c>
-      <c r="C11" t="n">
-        <v>54983</v>
-      </c>
-      <c r="D11" t="n">
-        <v>46575.88</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>39,962.00</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>59,040.00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>49,183.28</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2,459,164.00</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
-        <v>40162</v>
-      </c>
-      <c r="C12" t="n">
-        <v>57051</v>
-      </c>
-      <c r="D12" t="n">
-        <v>48813.38</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>40,071.00</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>59,040.00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>49,082.90</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2,454,145.00</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="n">
-        <v>41955</v>
-      </c>
-      <c r="C13" t="n">
-        <v>57051</v>
-      </c>
-      <c r="D13" t="n">
-        <v>49176.38</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>40,632.00</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>59,040.00</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>50,170.96</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2,508,548.00</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="n">
-        <v>41955</v>
-      </c>
-      <c r="C14" t="n">
-        <v>57051</v>
-      </c>
-      <c r="D14" t="n">
-        <v>50666.42</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>43,917.00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>59,040.00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>51,581.08</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2,579,054.00</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
-        <v>42597</v>
-      </c>
-      <c r="C15" t="n">
-        <v>58161</v>
-      </c>
-      <c r="D15" t="n">
-        <v>51980.82</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>42,470.00</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>59,040.00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>52,592.32</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2,629,616.00</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="n">
-        <v>44042</v>
-      </c>
-      <c r="C16" t="n">
-        <v>59214</v>
-      </c>
-      <c r="D16" t="n">
-        <v>52550.22</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>44,524.00</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>59,040.00</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>53,128.18</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2,656,409.00</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="n">
-        <v>45817</v>
-      </c>
-      <c r="C17" t="n">
-        <v>58671</v>
-      </c>
-      <c r="D17" t="n">
-        <v>53397.8</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>45,413.00</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>59,040.00</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>52,995.14</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2,649,757.00</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="n">
-        <v>47831</v>
-      </c>
-      <c r="C18" t="n">
-        <v>58671</v>
-      </c>
-      <c r="D18" t="n">
-        <v>54106.88</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>40,208.00</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>59,040.00</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>52,257.96</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2,612,898.00</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="n">
-        <v>47958</v>
-      </c>
-      <c r="C19" t="n">
-        <v>58671</v>
-      </c>
-      <c r="D19" t="n">
-        <v>54330.86</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>44,987.00</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>59,773.00</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>52,550.30</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2,627,515.00</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="n">
-        <v>47579</v>
-      </c>
-      <c r="C20" t="n">
-        <v>59341</v>
-      </c>
-      <c r="D20" t="n">
-        <v>54283.24</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>42,856.00</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>59,773.00</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>52,943.80</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2,647,190.00</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="n">
-        <v>47579</v>
-      </c>
-      <c r="C21" t="n">
-        <v>59341</v>
-      </c>
-      <c r="D21" t="n">
-        <v>54384.28</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>37,219.00</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>59,773.00</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>53,243.42</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2,662,171.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>44,622.00</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>59,773.00</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>54,280.62</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2,714,031.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>47,520.00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>61,171.00</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>54,637.40</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2,731,870.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>47,888.00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>61,171.00</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>54,839.28</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2,741,964.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>50,880.00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>61,171.00</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>55,523.30</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2,776,165.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>49,423.00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>61,171.00</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>56,267.98</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2,813,399.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>49,285.00</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>61,171.00</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>56,777.02</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2,838,851.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>50,251.00</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>61,171.00</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>57,945.18</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2,897,259.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>51,948.00</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>61,963.00</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>57,582.54</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2,879,127.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>52,224.00</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>62,135.00</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>57,603.88</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2,880,194.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>50,045.00</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>62,135.00</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>57,598.78</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2,879,939.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>52,719.00</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>62,135.00</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>58,092.04</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2,904,602.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>50,159.00</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>62,135.00</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>57,749.26</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2,887,463.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>50,766.00</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>62,135.00</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>57,738.88</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2,886,944.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>51,964.00</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>62,135.00</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>57,530.36</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2,876,518.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>52,401.00</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>62,135.00</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>58,078.38</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2,903,919.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>53,728.00</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>62,135.00</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>58,073.54</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2,903,677.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>55,271.00</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>63,343.00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>58,861.66</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2,943,083.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>53,494.00</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>63,343.00</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>59,078.80</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2,953,940.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>52,834.00</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>63,343.00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>59,250.46</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2,962,523.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>50,039.00</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>63,343.00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>59,349.00</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2,967,450.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>54,482.00</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>63,343.00</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>59,835.50</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2,991,775.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>55,773.00</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>63,995.00</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>60,119.26</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>3,005,963.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>55,963.00</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>63,995.00</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>60,237.34</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>3,011,867.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>53,485.00</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>64,673.00</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>60,551.32</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>3,027,566.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>54,961.00</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>65,209.00</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>60,612.42</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>3,030,621.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>55,734.00</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>65,209.00</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>61,141.38</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>3,057,069.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>56,648.00</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>65,209.00</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>61,055.14</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>3,052,757.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>56,607.00</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>65,209.00</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>61,135.64</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>3,056,782.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>55,724.00</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>66,938.00</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>61,297.32</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>3,064,866.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>58,231.00</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>66,938.00</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>61,741.10</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>3,087,055.00</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificaciones de parametros del AG
</commit_message>
<xml_diff>
--- a/Trabajo Practico Integrador/Salidas/Datos.xlsx
+++ b/Trabajo Practico Integrador/Salidas/Datos.xlsx
@@ -454,22 +454,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>36,581.00</t>
+          <t>14,454.00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>44,662.00</t>
+          <t>20,462.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>41,460.10</t>
+          <t>17,900.56</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2,073,005.00</t>
+          <t>895,028.00</t>
         </is>
       </c>
     </row>
@@ -479,22 +479,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>30,199.00</t>
+          <t>15,727.00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>50,983.00</t>
+          <t>20,905.00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>41,525.00</t>
+          <t>18,182.32</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2,076,250.00</t>
+          <t>909,116.00</t>
         </is>
       </c>
     </row>
@@ -504,22 +504,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>33,128.00</t>
+          <t>15,148.00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>50,983.00</t>
+          <t>20,905.00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>42,211.44</t>
+          <t>18,611.42</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2,110,572.00</t>
+          <t>930,571.00</t>
         </is>
       </c>
     </row>
@@ -529,22 +529,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>33,263.00</t>
+          <t>15,502.00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>54,124.00</t>
+          <t>20,905.00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>42,714.00</t>
+          <t>18,966.84</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2,135,700.00</t>
+          <t>948,342.00</t>
         </is>
       </c>
     </row>
@@ -554,22 +554,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>33,873.00</t>
+          <t>16,785.00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>54,124.00</t>
+          <t>20,905.00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>44,680.64</t>
+          <t>19,019.22</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2,234,032.00</t>
+          <t>950,961.00</t>
         </is>
       </c>
     </row>
@@ -579,22 +579,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>33,873.00</t>
+          <t>16,600.00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>56,689.00</t>
+          <t>21,024.00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>45,707.74</t>
+          <t>19,293.82</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2,285,387.00</t>
+          <t>964,691.00</t>
         </is>
       </c>
     </row>
@@ -604,22 +604,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>32,947.00</t>
+          <t>16,321.00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>56,689.00</t>
+          <t>21,024.00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>45,187.34</t>
+          <t>19,703.30</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2,259,367.00</t>
+          <t>985,165.00</t>
         </is>
       </c>
     </row>
@@ -629,22 +629,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>30,588.00</t>
+          <t>18,008.00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>58,349.00</t>
+          <t>21,816.00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>46,756.64</t>
+          <t>19,975.92</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2,337,832.00</t>
+          <t>998,796.00</t>
         </is>
       </c>
     </row>
@@ -654,22 +654,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>39,419.00</t>
+          <t>18,421.00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>58,349.00</t>
+          <t>22,077.00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>48,273.76</t>
+          <t>20,139.84</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2,413,688.00</t>
+          <t>1,006,992.00</t>
         </is>
       </c>
     </row>
@@ -679,22 +679,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>39,962.00</t>
+          <t>18,055.00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>59,040.00</t>
+          <t>22,478.00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>49,183.28</t>
+          <t>19,962.76</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2,459,164.00</t>
+          <t>998,138.00</t>
         </is>
       </c>
     </row>
@@ -704,22 +704,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>40,071.00</t>
+          <t>17,726.00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>59,040.00</t>
+          <t>22,478.00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>49,082.90</t>
+          <t>20,310.52</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2,454,145.00</t>
+          <t>1,015,526.00</t>
         </is>
       </c>
     </row>
@@ -729,22 +729,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>40,632.00</t>
+          <t>16,734.00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>59,040.00</t>
+          <t>22,478.00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>50,170.96</t>
+          <t>20,388.18</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2,508,548.00</t>
+          <t>1,019,409.00</t>
         </is>
       </c>
     </row>
@@ -754,22 +754,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>43,917.00</t>
+          <t>17,135.00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>59,040.00</t>
+          <t>22,478.00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>51,581.08</t>
+          <t>20,315.88</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2,579,054.00</t>
+          <t>1,015,794.00</t>
         </is>
       </c>
     </row>
@@ -779,22 +779,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>42,470.00</t>
+          <t>18,306.00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>59,040.00</t>
+          <t>22,718.00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>52,592.32</t>
+          <t>20,741.78</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2,629,616.00</t>
+          <t>1,037,089.00</t>
         </is>
       </c>
     </row>
@@ -804,22 +804,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>44,524.00</t>
+          <t>18,188.00</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>59,040.00</t>
+          <t>22,946.00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>53,128.18</t>
+          <t>20,882.82</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2,656,409.00</t>
+          <t>1,044,141.00</t>
         </is>
       </c>
     </row>
@@ -829,22 +829,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>45,413.00</t>
+          <t>18,698.00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>59,040.00</t>
+          <t>23,468.00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>52,995.14</t>
+          <t>21,114.92</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2,649,757.00</t>
+          <t>1,055,746.00</t>
         </is>
       </c>
     </row>
@@ -854,22 +854,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>40,208.00</t>
+          <t>19,293.00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>59,040.00</t>
+          <t>23,468.00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>52,257.96</t>
+          <t>21,059.70</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2,612,898.00</t>
+          <t>1,052,985.00</t>
         </is>
       </c>
     </row>
@@ -879,22 +879,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>44,987.00</t>
+          <t>18,848.00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>59,773.00</t>
+          <t>23,468.00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>52,550.30</t>
+          <t>21,341.04</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2,627,515.00</t>
+          <t>1,067,052.00</t>
         </is>
       </c>
     </row>
@@ -904,22 +904,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>42,856.00</t>
+          <t>19,750.00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>59,773.00</t>
+          <t>23,468.00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>52,943.80</t>
+          <t>21,666.50</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2,647,190.00</t>
+          <t>1,083,325.00</t>
         </is>
       </c>
     </row>
@@ -929,22 +929,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>37,219.00</t>
+          <t>19,868.00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>59,773.00</t>
+          <t>23,762.00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>53,243.42</t>
+          <t>21,828.74</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2,662,171.00</t>
+          <t>1,091,437.00</t>
         </is>
       </c>
     </row>
@@ -954,22 +954,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>44,622.00</t>
+          <t>19,288.00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>59,773.00</t>
+          <t>23,762.00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>54,280.62</t>
+          <t>21,958.68</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2,714,031.00</t>
+          <t>1,097,934.00</t>
         </is>
       </c>
     </row>
@@ -979,22 +979,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>47,520.00</t>
+          <t>19,578.00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>61,171.00</t>
+          <t>23,762.00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>54,637.40</t>
+          <t>21,986.54</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2,731,870.00</t>
+          <t>1,099,327.00</t>
         </is>
       </c>
     </row>
@@ -1004,22 +1004,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>47,888.00</t>
+          <t>19,344.00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>61,171.00</t>
+          <t>24,229.00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>54,839.28</t>
+          <t>22,007.46</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2,741,964.00</t>
+          <t>1,100,373.00</t>
         </is>
       </c>
     </row>
@@ -1029,22 +1029,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>50,880.00</t>
+          <t>18,283.00</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>61,171.00</t>
+          <t>24,229.00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>55,523.30</t>
+          <t>22,431.86</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2,776,165.00</t>
+          <t>1,121,593.00</t>
         </is>
       </c>
     </row>
@@ -1054,22 +1054,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>49,423.00</t>
+          <t>20,086.00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>61,171.00</t>
+          <t>24,229.00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>56,267.98</t>
+          <t>22,607.20</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2,813,399.00</t>
+          <t>1,130,360.00</t>
         </is>
       </c>
     </row>
@@ -1079,22 +1079,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>49,285.00</t>
+          <t>19,971.00</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>61,171.00</t>
+          <t>24,229.00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>56,777.02</t>
+          <t>22,532.94</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2,838,851.00</t>
+          <t>1,126,647.00</t>
         </is>
       </c>
     </row>
@@ -1104,22 +1104,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>50,251.00</t>
+          <t>19,690.00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>61,171.00</t>
+          <t>24,229.00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>57,945.18</t>
+          <t>22,467.70</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2,897,259.00</t>
+          <t>1,123,385.00</t>
         </is>
       </c>
     </row>
@@ -1129,22 +1129,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>51,948.00</t>
+          <t>20,476.00</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>61,963.00</t>
+          <t>24,296.00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>57,582.54</t>
+          <t>22,554.04</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2,879,127.00</t>
+          <t>1,127,702.00</t>
         </is>
       </c>
     </row>
@@ -1154,22 +1154,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>52,224.00</t>
+          <t>20,268.00</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>62,135.00</t>
+          <t>24,296.00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>57,603.88</t>
+          <t>22,490.06</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2,880,194.00</t>
+          <t>1,124,503.00</t>
         </is>
       </c>
     </row>
@@ -1179,22 +1179,22 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>50,045.00</t>
+          <t>20,539.00</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>62,135.00</t>
+          <t>24,521.00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>57,598.78</t>
+          <t>22,631.96</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2,879,939.00</t>
+          <t>1,131,598.00</t>
         </is>
       </c>
     </row>
@@ -1204,22 +1204,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>52,719.00</t>
+          <t>20,314.00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>62,135.00</t>
+          <t>24,691.00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>58,092.04</t>
+          <t>22,888.00</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2,904,602.00</t>
+          <t>1,144,400.00</t>
         </is>
       </c>
     </row>
@@ -1229,22 +1229,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>50,159.00</t>
+          <t>20,902.00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>62,135.00</t>
+          <t>24,691.00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>57,749.26</t>
+          <t>22,773.38</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2,887,463.00</t>
+          <t>1,138,669.00</t>
         </is>
       </c>
     </row>
@@ -1254,22 +1254,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>50,766.00</t>
+          <t>20,445.00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>62,135.00</t>
+          <t>24,691.00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>57,738.88</t>
+          <t>22,862.64</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2,886,944.00</t>
+          <t>1,143,132.00</t>
         </is>
       </c>
     </row>
@@ -1279,22 +1279,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>51,964.00</t>
+          <t>20,987.00</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>62,135.00</t>
+          <t>24,691.00</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>57,530.36</t>
+          <t>22,869.46</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2,876,518.00</t>
+          <t>1,143,473.00</t>
         </is>
       </c>
     </row>
@@ -1304,22 +1304,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>52,401.00</t>
+          <t>21,214.00</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>62,135.00</t>
+          <t>24,691.00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>58,078.38</t>
+          <t>23,245.76</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2,903,919.00</t>
+          <t>1,162,288.00</t>
         </is>
       </c>
     </row>
@@ -1329,22 +1329,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>53,728.00</t>
+          <t>21,466.00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>62,135.00</t>
+          <t>24,691.00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>58,073.54</t>
+          <t>23,094.94</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>2,903,677.00</t>
+          <t>1,154,747.00</t>
         </is>
       </c>
     </row>
@@ -1354,22 +1354,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>55,271.00</t>
+          <t>21,427.00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>63,343.00</t>
+          <t>24,691.00</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>58,861.66</t>
+          <t>23,125.72</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2,943,083.00</t>
+          <t>1,156,286.00</t>
         </is>
       </c>
     </row>
@@ -1379,22 +1379,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>53,494.00</t>
+          <t>20,964.00</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>63,343.00</t>
+          <t>24,691.00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>59,078.80</t>
+          <t>23,144.78</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2,953,940.00</t>
+          <t>1,157,239.00</t>
         </is>
       </c>
     </row>
@@ -1404,22 +1404,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>52,834.00</t>
+          <t>22,091.00</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>63,343.00</t>
+          <t>24,691.00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>59,250.46</t>
+          <t>23,261.16</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2,962,523.00</t>
+          <t>1,163,058.00</t>
         </is>
       </c>
     </row>
@@ -1429,22 +1429,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>50,039.00</t>
+          <t>21,209.00</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>63,343.00</t>
+          <t>24,691.00</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>59,349.00</t>
+          <t>23,090.44</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2,967,450.00</t>
+          <t>1,154,522.00</t>
         </is>
       </c>
     </row>
@@ -1454,22 +1454,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>54,482.00</t>
+          <t>21,673.00</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>63,343.00</t>
+          <t>24,815.00</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>59,835.50</t>
+          <t>23,248.28</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2,991,775.00</t>
+          <t>1,162,414.00</t>
         </is>
       </c>
     </row>
@@ -1479,22 +1479,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>55,773.00</t>
+          <t>21,777.00</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>63,995.00</t>
+          <t>24,815.00</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>60,119.26</t>
+          <t>23,215.60</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>3,005,963.00</t>
+          <t>1,160,780.00</t>
         </is>
       </c>
     </row>
@@ -1504,22 +1504,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>55,963.00</t>
+          <t>20,698.00</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>63,995.00</t>
+          <t>24,815.00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>60,237.34</t>
+          <t>23,360.08</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>3,011,867.00</t>
+          <t>1,168,004.00</t>
         </is>
       </c>
     </row>
@@ -1529,22 +1529,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>53,485.00</t>
+          <t>21,852.00</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>64,673.00</t>
+          <t>25,109.00</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>60,551.32</t>
+          <t>23,360.00</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>3,027,566.00</t>
+          <t>1,168,000.00</t>
         </is>
       </c>
     </row>
@@ -1554,22 +1554,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>54,961.00</t>
+          <t>22,094.00</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>65,209.00</t>
+          <t>25,109.00</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>60,612.42</t>
+          <t>23,460.06</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>3,030,621.00</t>
+          <t>1,173,003.00</t>
         </is>
       </c>
     </row>
@@ -1579,22 +1579,22 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>55,734.00</t>
+          <t>21,728.00</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>65,209.00</t>
+          <t>25,109.00</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>61,141.38</t>
+          <t>23,484.10</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>3,057,069.00</t>
+          <t>1,174,205.00</t>
         </is>
       </c>
     </row>
@@ -1604,22 +1604,22 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>56,648.00</t>
+          <t>21,358.00</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>65,209.00</t>
+          <t>25,109.00</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>61,055.14</t>
+          <t>23,546.54</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>3,052,757.00</t>
+          <t>1,177,327.00</t>
         </is>
       </c>
     </row>
@@ -1629,22 +1629,22 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>56,607.00</t>
+          <t>21,892.00</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>65,209.00</t>
+          <t>25,132.00</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>61,135.64</t>
+          <t>23,591.64</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>3,056,782.00</t>
+          <t>1,179,582.00</t>
         </is>
       </c>
     </row>
@@ -1654,22 +1654,22 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>55,724.00</t>
+          <t>20,444.00</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>66,938.00</t>
+          <t>25,132.00</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>61,297.32</t>
+          <t>23,585.04</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>3,064,866.00</t>
+          <t>1,179,252.00</t>
         </is>
       </c>
     </row>
@@ -1679,22 +1679,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>58,231.00</t>
+          <t>21,148.00</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>66,938.00</t>
+          <t>25,132.00</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>61,741.10</t>
+          <t>23,730.06</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>3,087,055.00</t>
+          <t>1,186,503.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Eliminacion de libreria enum, sin uso
</commit_message>
<xml_diff>
--- a/Trabajo Practico Integrador/Salidas/Datos.xlsx
+++ b/Trabajo Practico Integrador/Salidas/Datos.xlsx
@@ -454,22 +454,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14,454.00</t>
+          <t>12,151.00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>20,462.00</t>
+          <t>16,882.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>17,900.56</t>
+          <t>15,055.38</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>895,028.00</t>
+          <t>752,769.00</t>
         </is>
       </c>
     </row>
@@ -479,22 +479,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15,727.00</t>
+          <t>12,384.00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20,905.00</t>
+          <t>16,882.00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>18,182.32</t>
+          <t>14,912.80</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>909,116.00</t>
+          <t>745,640.00</t>
         </is>
       </c>
     </row>
@@ -504,22 +504,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>15,148.00</t>
+          <t>12,148.00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>20,905.00</t>
+          <t>16,934.00</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18,611.42</t>
+          <t>14,870.38</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>930,571.00</t>
+          <t>743,519.00</t>
         </is>
       </c>
     </row>
@@ -529,22 +529,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15,502.00</t>
+          <t>12,117.00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>20,905.00</t>
+          <t>16,934.00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>18,966.84</t>
+          <t>15,078.40</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>948,342.00</t>
+          <t>753,920.00</t>
         </is>
       </c>
     </row>
@@ -554,22 +554,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16,785.00</t>
+          <t>13,257.00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>20,905.00</t>
+          <t>17,489.00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>19,019.22</t>
+          <t>15,529.62</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>950,961.00</t>
+          <t>776,481.00</t>
         </is>
       </c>
     </row>
@@ -579,22 +579,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16,600.00</t>
+          <t>13,978.00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>21,024.00</t>
+          <t>18,454.00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>19,293.82</t>
+          <t>15,967.46</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>964,691.00</t>
+          <t>798,373.00</t>
         </is>
       </c>
     </row>
@@ -604,22 +604,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16,321.00</t>
+          <t>14,128.00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>21,024.00</t>
+          <t>18,633.00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>19,703.30</t>
+          <t>16,282.16</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>985,165.00</t>
+          <t>814,108.00</t>
         </is>
       </c>
     </row>
@@ -629,22 +629,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>18,008.00</t>
+          <t>13,105.00</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>21,816.00</t>
+          <t>18,747.00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>19,975.92</t>
+          <t>16,551.86</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>998,796.00</t>
+          <t>827,593.00</t>
         </is>
       </c>
     </row>
@@ -654,22 +654,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>18,421.00</t>
+          <t>13,818.00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>22,077.00</t>
+          <t>18,747.00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>20,139.84</t>
+          <t>16,474.62</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1,006,992.00</t>
+          <t>823,731.00</t>
         </is>
       </c>
     </row>
@@ -679,22 +679,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>18,055.00</t>
+          <t>14,041.00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>22,478.00</t>
+          <t>18,747.00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>19,962.76</t>
+          <t>16,851.14</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>998,138.00</t>
+          <t>842,557.00</t>
         </is>
       </c>
     </row>
@@ -704,22 +704,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17,726.00</t>
+          <t>14,606.00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>22,478.00</t>
+          <t>18,747.00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>20,310.52</t>
+          <t>16,831.32</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1,015,526.00</t>
+          <t>841,566.00</t>
         </is>
       </c>
     </row>
@@ -729,22 +729,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16,734.00</t>
+          <t>14,726.00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>22,478.00</t>
+          <t>18,963.00</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>20,388.18</t>
+          <t>16,980.56</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1,019,409.00</t>
+          <t>849,028.00</t>
         </is>
       </c>
     </row>
@@ -754,22 +754,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>17,135.00</t>
+          <t>14,920.00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>22,478.00</t>
+          <t>18,963.00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>20,315.88</t>
+          <t>16,858.60</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1,015,794.00</t>
+          <t>842,930.00</t>
         </is>
       </c>
     </row>
@@ -779,22 +779,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>18,306.00</t>
+          <t>14,393.00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>22,718.00</t>
+          <t>18,963.00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>20,741.78</t>
+          <t>16,997.54</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1,037,089.00</t>
+          <t>849,877.00</t>
         </is>
       </c>
     </row>
@@ -804,22 +804,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>18,188.00</t>
+          <t>14,632.00</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>22,946.00</t>
+          <t>18,963.00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>20,882.82</t>
+          <t>17,103.64</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1,044,141.00</t>
+          <t>855,182.00</t>
         </is>
       </c>
     </row>
@@ -829,22 +829,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>18,698.00</t>
+          <t>15,022.00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>23,468.00</t>
+          <t>19,133.00</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>21,114.92</t>
+          <t>17,261.18</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1,055,746.00</t>
+          <t>863,059.00</t>
         </is>
       </c>
     </row>
@@ -854,22 +854,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>19,293.00</t>
+          <t>15,092.00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>23,468.00</t>
+          <t>19,133.00</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>21,059.70</t>
+          <t>17,233.20</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1,052,985.00</t>
+          <t>861,660.00</t>
         </is>
       </c>
     </row>
@@ -879,22 +879,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>18,848.00</t>
+          <t>15,556.00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>23,468.00</t>
+          <t>19,133.00</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>21,341.04</t>
+          <t>17,189.40</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1,067,052.00</t>
+          <t>859,470.00</t>
         </is>
       </c>
     </row>
@@ -904,22 +904,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>19,750.00</t>
+          <t>15,265.00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>23,468.00</t>
+          <t>19,133.00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>21,666.50</t>
+          <t>17,226.14</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1,083,325.00</t>
+          <t>861,307.00</t>
         </is>
       </c>
     </row>
@@ -929,22 +929,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>19,868.00</t>
+          <t>15,265.00</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>23,762.00</t>
+          <t>19,133.00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>21,828.74</t>
+          <t>17,412.74</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1,091,437.00</t>
+          <t>870,637.00</t>
         </is>
       </c>
     </row>
@@ -954,22 +954,22 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>19,288.00</t>
+          <t>16,019.00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>23,762.00</t>
+          <t>19,133.00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>21,958.68</t>
+          <t>17,524.00</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1,097,934.00</t>
+          <t>876,200.00</t>
         </is>
       </c>
     </row>
@@ -979,22 +979,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>19,578.00</t>
+          <t>15,670.00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>23,762.00</t>
+          <t>19,391.00</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>21,986.54</t>
+          <t>17,622.30</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1,099,327.00</t>
+          <t>881,115.00</t>
         </is>
       </c>
     </row>
@@ -1004,22 +1004,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>19,344.00</t>
+          <t>15,851.00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>24,229.00</t>
+          <t>19,391.00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>22,007.46</t>
+          <t>17,528.14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1,100,373.00</t>
+          <t>876,407.00</t>
         </is>
       </c>
     </row>
@@ -1029,22 +1029,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>18,283.00</t>
+          <t>15,243.00</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>24,229.00</t>
+          <t>19,391.00</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>22,431.86</t>
+          <t>17,614.60</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1,121,593.00</t>
+          <t>880,730.00</t>
         </is>
       </c>
     </row>
@@ -1054,22 +1054,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>20,086.00</t>
+          <t>15,367.00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>24,229.00</t>
+          <t>19,391.00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>22,607.20</t>
+          <t>17,682.76</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1,130,360.00</t>
+          <t>884,138.00</t>
         </is>
       </c>
     </row>
@@ -1079,22 +1079,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>19,971.00</t>
+          <t>16,405.00</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>24,229.00</t>
+          <t>19,396.00</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>22,532.94</t>
+          <t>17,740.38</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1,126,647.00</t>
+          <t>887,019.00</t>
         </is>
       </c>
     </row>
@@ -1104,22 +1104,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>19,690.00</t>
+          <t>15,975.00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>24,229.00</t>
+          <t>19,396.00</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>22,467.70</t>
+          <t>17,896.24</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1,123,385.00</t>
+          <t>894,812.00</t>
         </is>
       </c>
     </row>
@@ -1129,22 +1129,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>20,476.00</t>
+          <t>15,266.00</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>24,296.00</t>
+          <t>19,396.00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>22,554.04</t>
+          <t>17,773.72</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1,127,702.00</t>
+          <t>888,686.00</t>
         </is>
       </c>
     </row>
@@ -1154,22 +1154,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>20,268.00</t>
+          <t>16,070.00</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>24,296.00</t>
+          <t>19,396.00</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>22,490.06</t>
+          <t>17,743.22</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1,124,503.00</t>
+          <t>887,161.00</t>
         </is>
       </c>
     </row>
@@ -1179,22 +1179,22 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>20,539.00</t>
+          <t>15,846.00</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>24,521.00</t>
+          <t>19,396.00</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>22,631.96</t>
+          <t>17,753.18</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1,131,598.00</t>
+          <t>887,659.00</t>
         </is>
       </c>
     </row>
@@ -1204,22 +1204,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>20,314.00</t>
+          <t>16,341.00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>24,691.00</t>
+          <t>19,396.00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>22,888.00</t>
+          <t>17,778.60</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1,144,400.00</t>
+          <t>888,930.00</t>
         </is>
       </c>
     </row>
@@ -1229,22 +1229,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>20,902.00</t>
+          <t>16,353.00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>24,691.00</t>
+          <t>19,396.00</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>22,773.38</t>
+          <t>17,831.64</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1,138,669.00</t>
+          <t>891,582.00</t>
         </is>
       </c>
     </row>
@@ -1254,22 +1254,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>20,445.00</t>
+          <t>16,601.00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>24,691.00</t>
+          <t>19,396.00</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>22,862.64</t>
+          <t>18,003.22</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1,143,132.00</t>
+          <t>900,161.00</t>
         </is>
       </c>
     </row>
@@ -1279,22 +1279,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>20,987.00</t>
+          <t>16,656.00</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>24,691.00</t>
+          <t>19,396.00</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>22,869.46</t>
+          <t>18,037.08</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1,143,473.00</t>
+          <t>901,854.00</t>
         </is>
       </c>
     </row>
@@ -1304,22 +1304,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>21,214.00</t>
+          <t>16,696.00</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>24,691.00</t>
+          <t>19,396.00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>23,245.76</t>
+          <t>18,061.48</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1,162,288.00</t>
+          <t>903,074.00</t>
         </is>
       </c>
     </row>
@@ -1329,22 +1329,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>21,466.00</t>
+          <t>16,826.00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>24,691.00</t>
+          <t>19,396.00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>23,094.94</t>
+          <t>18,271.08</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1,154,747.00</t>
+          <t>913,554.00</t>
         </is>
       </c>
     </row>
@@ -1354,22 +1354,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>21,427.00</t>
+          <t>16,635.00</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>24,691.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>23,125.72</t>
+          <t>18,519.64</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1,156,286.00</t>
+          <t>925,982.00</t>
         </is>
       </c>
     </row>
@@ -1379,22 +1379,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>20,964.00</t>
+          <t>17,005.00</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>24,691.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>23,144.78</t>
+          <t>18,502.72</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1,157,239.00</t>
+          <t>925,136.00</t>
         </is>
       </c>
     </row>
@@ -1404,22 +1404,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>22,091.00</t>
+          <t>17,051.00</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>24,691.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>23,261.16</t>
+          <t>18,445.68</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1,163,058.00</t>
+          <t>922,284.00</t>
         </is>
       </c>
     </row>
@@ -1429,22 +1429,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>21,209.00</t>
+          <t>16,826.00</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>24,691.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>23,090.44</t>
+          <t>18,437.30</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1,154,522.00</t>
+          <t>921,865.00</t>
         </is>
       </c>
     </row>
@@ -1454,22 +1454,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>21,673.00</t>
+          <t>16,780.00</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>24,815.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>23,248.28</t>
+          <t>18,572.74</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1,162,414.00</t>
+          <t>928,637.00</t>
         </is>
       </c>
     </row>
@@ -1479,22 +1479,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>21,777.00</t>
+          <t>16,610.00</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>24,815.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>23,215.60</t>
+          <t>18,485.92</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1,160,780.00</t>
+          <t>924,296.00</t>
         </is>
       </c>
     </row>
@@ -1504,22 +1504,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>20,698.00</t>
+          <t>16,494.00</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>24,815.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>23,360.08</t>
+          <t>18,520.18</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1,168,004.00</t>
+          <t>926,009.00</t>
         </is>
       </c>
     </row>
@@ -1529,22 +1529,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>21,852.00</t>
+          <t>16,008.00</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>25,109.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>23,360.00</t>
+          <t>18,567.48</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1,168,000.00</t>
+          <t>928,374.00</t>
         </is>
       </c>
     </row>
@@ -1554,22 +1554,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>22,094.00</t>
+          <t>16,301.00</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>25,109.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>23,460.06</t>
+          <t>18,479.66</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1,173,003.00</t>
+          <t>923,983.00</t>
         </is>
       </c>
     </row>
@@ -1579,22 +1579,22 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>21,728.00</t>
+          <t>16,661.00</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>25,109.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>23,484.10</t>
+          <t>18,446.74</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1,174,205.00</t>
+          <t>922,337.00</t>
         </is>
       </c>
     </row>
@@ -1604,22 +1604,22 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>21,358.00</t>
+          <t>16,179.00</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>25,109.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>23,546.54</t>
+          <t>18,423.80</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1,177,327.00</t>
+          <t>921,190.00</t>
         </is>
       </c>
     </row>
@@ -1629,22 +1629,22 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>21,892.00</t>
+          <t>17,053.00</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>25,132.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>23,591.64</t>
+          <t>18,458.60</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1,179,582.00</t>
+          <t>922,930.00</t>
         </is>
       </c>
     </row>
@@ -1654,22 +1654,22 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>20,444.00</t>
+          <t>15,960.00</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>25,132.00</t>
+          <t>19,442.00</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>23,585.04</t>
+          <t>18,423.38</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1,179,252.00</t>
+          <t>921,169.00</t>
         </is>
       </c>
     </row>
@@ -1679,22 +1679,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>21,148.00</t>
+          <t>16,920.00</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>25,132.00</t>
+          <t>19,667.00</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>23,730.06</t>
+          <t>18,492.22</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1,186,503.00</t>
+          <t>924,611.00</t>
         </is>
       </c>
     </row>

</xml_diff>